<commit_message>
Update demographics Medication information for MDD for fMRI Analysis
</commit_message>
<xml_diff>
--- a/data/Demographics.xlsx
+++ b/data/Demographics.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="239">
   <si>
     <t>Healthy Control (HC) or Patient</t>
   </si>
@@ -901,12 +901,15 @@
   <si>
     <t>NaN</t>
   </si>
+  <si>
+    <t>Bids-Nummer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -995,8 +998,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1045,6 +1058,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6A6A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1076,7 +1095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1167,6 +1186,21 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5297,7 +5331,7 @@
   <dimension ref="A1:K128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15.75"/>
@@ -9758,68 +9792,71 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K117"/>
+  <dimension ref="A1:L130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="24.375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="53.125" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="9.125" style="4"/>
+    <col min="1" max="1" width="12.25" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="4" customWidth="1"/>
+    <col min="8" max="8" width="9" style="4" customWidth="1"/>
+    <col min="9" max="9" width="11.875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="24.375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="53.125" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="9.125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:12" s="19" customFormat="1" ht="30">
+      <c r="A1" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>0</v>
-      </c>
       <c r="G1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="L1" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="15">
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="15">
@@ -9828,31 +9865,34 @@
       <c r="E2" s="15">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
+      <c r="F2" s="15">
+        <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2">
         <v>23</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A3" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="15">
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="15">
@@ -9861,31 +9901,34 @@
       <c r="E3" s="15">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
+      <c r="F3" s="15">
+        <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="2">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="2">
         <v>19</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="4"/>
+      <c r="K3" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="15">
+      <c r="B4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="15">
@@ -9894,31 +9937,34 @@
       <c r="E4" s="15">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
+      <c r="F4" s="15">
+        <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="2">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2">
         <v>27</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="4"/>
+      <c r="K4" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A5" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="15">
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="15">
@@ -9927,1707 +9973,2391 @@
       <c r="E5" s="15">
         <v>1</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
+      <c r="F5" s="15">
+        <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="2">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2">
         <v>36</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="4"/>
+      <c r="K5" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A6" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="2">
+        <v>32</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A7" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6" s="15">
-        <v>1</v>
-      </c>
-      <c r="D6" s="15">
-        <v>1</v>
-      </c>
-      <c r="E6" s="15">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="B7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1</v>
+      </c>
+      <c r="E7" s="15">
+        <v>1</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="2">
         <v>26</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="2" t="s">
+      <c r="J7" s="4"/>
+      <c r="K7" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A7" s="9" t="s">
+    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A8" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="15">
-        <v>1</v>
-      </c>
-      <c r="D7" s="15">
-        <v>1</v>
-      </c>
-      <c r="E7" s="15">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="B8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15">
+        <v>1</v>
+      </c>
+      <c r="F8" s="15">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="2">
         <v>30</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="2" t="s">
+      <c r="J8" s="4"/>
+      <c r="K8" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A9" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="15">
-        <v>1</v>
-      </c>
-      <c r="D8" s="15">
-        <v>1</v>
-      </c>
-      <c r="E8" s="15">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="B9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="2">
         <v>18</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="2" t="s">
+      <c r="J9" s="4"/>
+      <c r="K9" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A9" s="9" t="s">
+    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A10" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15">
-        <v>1</v>
-      </c>
-      <c r="D9" s="15">
-        <v>1</v>
-      </c>
-      <c r="E9" s="15">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="2">
+      <c r="B10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="2">
         <v>30</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="2" t="s">
+      <c r="J10" s="4"/>
+      <c r="K10" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A11" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15">
-        <v>1</v>
-      </c>
-      <c r="D10" s="15">
-        <v>1</v>
-      </c>
-      <c r="E10" s="15">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="2">
+      <c r="B11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15">
+        <v>1</v>
+      </c>
+      <c r="F11" s="15">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="2">
         <v>38</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="2" t="s">
+      <c r="J11" s="4"/>
+      <c r="K11" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A11" s="9" t="s">
+    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A12" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="15">
-        <v>1</v>
-      </c>
-      <c r="D11" s="15">
-        <v>1</v>
-      </c>
-      <c r="E11" s="15">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="B12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1</v>
+      </c>
+      <c r="E12" s="15">
+        <v>1</v>
+      </c>
+      <c r="F12" s="15">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="2">
         <v>21</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="2" t="s">
+      <c r="J12" s="4"/>
+      <c r="K12" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A12" s="9" t="s">
+    <row r="13" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A13" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C12" s="15">
-        <v>1</v>
-      </c>
-      <c r="D12" s="15">
-        <v>1</v>
-      </c>
-      <c r="E12" s="15">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="D13" s="15">
+        <v>1</v>
+      </c>
+      <c r="E13" s="15">
+        <v>1</v>
+      </c>
+      <c r="F13" s="15">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="2">
         <v>27</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="2" t="s">
+      <c r="J13" s="4"/>
+      <c r="K13" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A13" s="9" t="s">
+    <row r="14" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A14" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="15">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="2">
+        <v>27</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A15" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="15">
-        <v>1</v>
-      </c>
-      <c r="D13" s="15">
-        <v>1</v>
-      </c>
-      <c r="E13" s="15">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="2">
+      <c r="B15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="2">
         <v>36</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="2" t="s">
+      <c r="J15" s="4"/>
+      <c r="K15" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A14" s="9" t="s">
+    <row r="16" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A16" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="15">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="2">
+        <v>21</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A17" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="15">
-        <v>1</v>
-      </c>
-      <c r="D14" s="15">
-        <v>1</v>
-      </c>
-      <c r="E14" s="15">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="2">
+      <c r="B17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1</v>
+      </c>
+      <c r="E17" s="15">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="2">
         <v>28</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="2" t="s">
+      <c r="J17" s="4"/>
+      <c r="K17" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="9" t="s">
+    <row r="18" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A18" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="2">
+        <v>41</v>
+      </c>
+      <c r="J18" s="4"/>
+      <c r="K18" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A19" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="2">
-        <v>0</v>
-      </c>
-      <c r="C15" s="15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="15">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="2">
+      <c r="B19" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="15">
+        <v>1</v>
+      </c>
+      <c r="E19" s="15">
+        <v>1</v>
+      </c>
+      <c r="F19" s="15">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="2">
         <v>22</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="2" t="s">
+      <c r="J19" s="4"/>
+      <c r="K19" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A16" s="9" t="s">
+    <row r="20" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A20" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" s="15">
-        <v>1</v>
-      </c>
-      <c r="D16" s="15">
-        <v>1</v>
-      </c>
-      <c r="E16" s="15">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="2">
+      <c r="B20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1</v>
+      </c>
+      <c r="E20" s="15">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="2">
         <v>26</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="2" t="s">
+      <c r="J20" s="4"/>
+      <c r="K20" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A17" s="12" t="s">
+    <row r="21" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A21" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17" s="15">
-        <v>1</v>
-      </c>
-      <c r="D17" s="15">
-        <v>1</v>
-      </c>
-      <c r="E17" s="15">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="2">
+      <c r="B21" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="D21" s="15">
+        <v>1</v>
+      </c>
+      <c r="E21" s="15">
+        <v>1</v>
+      </c>
+      <c r="F21" s="15">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="2">
         <v>18</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="2" t="s">
+      <c r="J21" s="4"/>
+      <c r="K21" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A18" s="9" t="s">
+    <row r="22" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A22" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="15">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="2">
+        <v>37</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A23" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="15">
-        <v>1</v>
-      </c>
-      <c r="D18" s="15">
-        <v>1</v>
-      </c>
-      <c r="E18" s="15">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="2">
+      <c r="B23" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="15">
+        <v>1</v>
+      </c>
+      <c r="E23" s="15">
+        <v>1</v>
+      </c>
+      <c r="F23" s="15">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="2">
         <v>18</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="2" t="s">
+      <c r="J23" s="4"/>
+      <c r="K23" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A19" s="9" t="s">
+    <row r="24" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A24" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="15">
-        <v>1</v>
-      </c>
-      <c r="D19" s="15">
-        <v>1</v>
-      </c>
-      <c r="E19" s="15">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="2">
+      <c r="B24" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
+      <c r="D24" s="15">
+        <v>1</v>
+      </c>
+      <c r="E24" s="15">
+        <v>1</v>
+      </c>
+      <c r="F24" s="15">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="2">
         <v>39</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="2" t="s">
+      <c r="J24" s="4"/>
+      <c r="K24" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A20" s="9" t="s">
+    <row r="25" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A25" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="2">
-        <v>0</v>
-      </c>
-      <c r="C20" s="15">
-        <v>1</v>
-      </c>
-      <c r="D20" s="15">
-        <v>1</v>
-      </c>
-      <c r="E20" s="15">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="2">
+      <c r="B25" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="15">
+        <v>1</v>
+      </c>
+      <c r="E25" s="15">
+        <v>1</v>
+      </c>
+      <c r="F25" s="15">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="2">
         <v>22</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="2" t="s">
+      <c r="J25" s="4"/>
+      <c r="K25" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A21" s="9" t="s">
+    <row r="26" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A26" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="2">
-        <v>0</v>
-      </c>
-      <c r="C21" s="15">
-        <v>1</v>
-      </c>
-      <c r="D21" s="15">
-        <v>1</v>
-      </c>
-      <c r="E21" s="15">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="2">
+      <c r="B26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="D26" s="15">
+        <v>1</v>
+      </c>
+      <c r="E26" s="15">
+        <v>1</v>
+      </c>
+      <c r="F26" s="15">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="2">
         <v>23</v>
       </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A22" s="9" t="s">
+      <c r="J26" s="4"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A27" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="15">
-        <v>1</v>
-      </c>
-      <c r="D22" s="15">
-        <v>1</v>
-      </c>
-      <c r="E22" s="15">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="2">
+      <c r="B27" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="15">
+        <v>1</v>
+      </c>
+      <c r="E27" s="15">
+        <v>1</v>
+      </c>
+      <c r="F27" s="15">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="2">
         <v>32</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="2" t="s">
+      <c r="J27" s="4"/>
+      <c r="K27" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L27" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A23" s="9" t="s">
+    <row r="28" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A28" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
-      <c r="C23" s="15">
-        <v>1</v>
-      </c>
-      <c r="D23" s="15">
-        <v>1</v>
-      </c>
-      <c r="E23" s="15">
-        <v>1</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="2">
+      <c r="B28" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="15">
+        <v>1</v>
+      </c>
+      <c r="E28" s="15">
+        <v>1</v>
+      </c>
+      <c r="F28" s="15">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="2">
         <v>27</v>
       </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="2" t="s">
+      <c r="J28" s="4"/>
+      <c r="K28" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L28" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A24" s="9" t="s">
+    <row r="29" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A29" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
-      <c r="C24" s="15">
-        <v>1</v>
-      </c>
-      <c r="D24" s="15">
-        <v>1</v>
-      </c>
-      <c r="E24" s="15">
-        <v>1</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="2">
+      <c r="B29" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="15">
+        <v>1</v>
+      </c>
+      <c r="E29" s="15">
+        <v>1</v>
+      </c>
+      <c r="F29" s="15">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="2">
         <v>20</v>
       </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="2" t="s">
+      <c r="J29" s="4"/>
+      <c r="K29" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A25" s="13" t="s">
+    <row r="30" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A30" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
+      <c r="E30" s="15">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="2">
+        <v>21</v>
+      </c>
+      <c r="J30" s="4"/>
+      <c r="K30" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A31" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="15">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="2">
+        <v>22</v>
+      </c>
+      <c r="J31" s="4"/>
+      <c r="K31" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A32" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
+      <c r="D32" s="15">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="2">
+        <v>20</v>
+      </c>
+      <c r="J32" s="4"/>
+      <c r="K32" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A33" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="15">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="2">
+        <v>25</v>
+      </c>
+      <c r="J33" s="4"/>
+      <c r="K33" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A34" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="2">
-        <v>1</v>
-      </c>
-      <c r="C25" s="15">
-        <v>1</v>
-      </c>
-      <c r="D25" s="15">
-        <v>1</v>
-      </c>
-      <c r="E25" s="15">
-        <v>1</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" s="2">
+      <c r="B34" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1</v>
+      </c>
+      <c r="D34" s="15">
+        <v>1</v>
+      </c>
+      <c r="E34" s="15">
+        <v>1</v>
+      </c>
+      <c r="F34" s="15">
+        <v>1</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="2">
         <v>22</v>
       </c>
-      <c r="I25" s="4"/>
-      <c r="J25" s="2" t="s">
+      <c r="J34" s="4"/>
+      <c r="K34" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="L34" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A26" s="13" t="s">
+    <row r="35" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A35" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="2">
-        <v>0</v>
-      </c>
-      <c r="C26" s="15">
-        <v>1</v>
-      </c>
-      <c r="D26" s="15">
-        <v>1</v>
-      </c>
-      <c r="E26" s="15">
-        <v>1</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="2">
+      <c r="B35" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="D35" s="15">
+        <v>1</v>
+      </c>
+      <c r="E35" s="15">
+        <v>1</v>
+      </c>
+      <c r="F35" s="15">
+        <v>1</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" s="2">
         <v>25</v>
       </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="2" t="s">
+      <c r="J35" s="4"/>
+      <c r="K35" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="L35" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A27" s="13" t="s">
+    <row r="36" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A36" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="B27" s="2">
-        <v>0</v>
-      </c>
-      <c r="C27" s="15">
-        <v>1</v>
-      </c>
-      <c r="D27" s="15">
-        <v>1</v>
-      </c>
-      <c r="E27" s="15">
-        <v>1</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" s="2">
+      <c r="B36" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="D36" s="15">
+        <v>1</v>
+      </c>
+      <c r="E36" s="15">
+        <v>1</v>
+      </c>
+      <c r="F36" s="15">
+        <v>1</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="2">
         <v>31</v>
       </c>
-      <c r="I27" s="4"/>
-      <c r="J27" s="2" t="s">
+      <c r="J36" s="4"/>
+      <c r="K36" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="K27" s="10" t="s">
+      <c r="L36" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A28" s="13" t="s">
+    <row r="37" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A37" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="B28" s="2">
-        <v>0</v>
-      </c>
-      <c r="C28" s="15">
-        <v>1</v>
-      </c>
-      <c r="D28" s="15">
-        <v>1</v>
-      </c>
-      <c r="E28" s="15">
-        <v>1</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" s="2">
+      <c r="B37" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="D37" s="15">
+        <v>1</v>
+      </c>
+      <c r="E37" s="15">
+        <v>1</v>
+      </c>
+      <c r="F37" s="15">
+        <v>1</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="2">
         <v>27</v>
       </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A29" s="13" t="s">
+      <c r="J37" s="4"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A38" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
-      <c r="C29" s="15">
-        <v>1</v>
-      </c>
-      <c r="D29" s="15">
-        <v>1</v>
-      </c>
-      <c r="E29" s="15">
-        <v>1</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" s="2">
+      <c r="B38" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1</v>
+      </c>
+      <c r="D38" s="15">
+        <v>1</v>
+      </c>
+      <c r="E38" s="15">
+        <v>1</v>
+      </c>
+      <c r="F38" s="15">
+        <v>1</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I38" s="2">
         <v>22</v>
       </c>
-      <c r="I29" s="4"/>
-      <c r="J29" s="2" t="s">
+      <c r="J38" s="4"/>
+      <c r="K38" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="L38" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A30" s="13" t="s">
+    <row r="39" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A39" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="B30" s="2">
-        <v>0</v>
-      </c>
-      <c r="C30" s="15">
-        <v>1</v>
-      </c>
-      <c r="D30" s="15">
-        <v>1</v>
-      </c>
-      <c r="E30" s="15">
-        <v>1</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="2">
+      <c r="B39" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="D39" s="15">
+        <v>1</v>
+      </c>
+      <c r="E39" s="15">
+        <v>1</v>
+      </c>
+      <c r="F39" s="15">
+        <v>1</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="2">
         <v>28</v>
       </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="2" t="s">
+      <c r="J39" s="4"/>
+      <c r="K39" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K30" s="4" t="s">
+      <c r="L39" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A31" s="13" t="s">
+    <row r="40" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A40" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" s="15">
-        <v>1</v>
-      </c>
-      <c r="D31" s="15">
-        <v>1</v>
-      </c>
-      <c r="E31" s="15">
-        <v>1</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="4">
+      <c r="B40" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C40" s="4">
+        <v>1</v>
+      </c>
+      <c r="D40" s="15">
+        <v>1</v>
+      </c>
+      <c r="E40" s="15">
+        <v>1</v>
+      </c>
+      <c r="F40" s="15">
+        <v>1</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="4">
         <v>21</v>
       </c>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4" t="s">
+      <c r="J40" s="4"/>
+      <c r="K40" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="L40" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A32" s="13" t="s">
+    <row r="41" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A41" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" s="15">
-        <v>1</v>
-      </c>
-      <c r="D32" s="15">
-        <v>1</v>
-      </c>
-      <c r="E32" s="15">
-        <v>1</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="4">
+      <c r="B41" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" s="4">
+        <v>1</v>
+      </c>
+      <c r="D41" s="15">
+        <v>1</v>
+      </c>
+      <c r="E41" s="15">
+        <v>1</v>
+      </c>
+      <c r="F41" s="15">
+        <v>1</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I41" s="4">
         <v>34</v>
       </c>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4" t="s">
+      <c r="J41" s="4"/>
+      <c r="K41" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="L41" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A33" s="13" t="s">
+    <row r="42" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A42" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="B33" s="4">
-        <v>1</v>
-      </c>
-      <c r="C33" s="15">
-        <v>1</v>
-      </c>
-      <c r="D33" s="15">
-        <v>1</v>
-      </c>
-      <c r="E33" s="15">
-        <v>1</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H33" s="4">
+      <c r="B42" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
+      <c r="D42" s="15">
+        <v>1</v>
+      </c>
+      <c r="E42" s="15">
+        <v>1</v>
+      </c>
+      <c r="F42" s="15">
+        <v>1</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="4">
         <v>26</v>
       </c>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4" t="s">
+      <c r="J42" s="4"/>
+      <c r="K42" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="L42" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A34" s="13" t="s">
+    <row r="43" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A43" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="B34" s="14">
-        <v>1</v>
-      </c>
-      <c r="C34" s="15">
-        <v>1</v>
-      </c>
-      <c r="D34" s="15">
-        <v>1</v>
-      </c>
-      <c r="E34" s="15">
-        <v>1</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" s="14">
+      <c r="B43" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C43" s="14">
+        <v>1</v>
+      </c>
+      <c r="D43" s="15">
+        <v>1</v>
+      </c>
+      <c r="E43" s="15">
+        <v>1</v>
+      </c>
+      <c r="F43" s="15">
+        <v>1</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="14">
         <v>22</v>
       </c>
-      <c r="I34" s="4"/>
-      <c r="J34" s="14" t="s">
+      <c r="J43" s="4"/>
+      <c r="K43" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="K34" s="14" t="s">
+      <c r="L43" s="14" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A35" s="13" t="s">
+    <row r="44" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A44" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="B35" s="14">
-        <v>1</v>
-      </c>
-      <c r="C35" s="15">
-        <v>1</v>
-      </c>
-      <c r="D35" s="15">
-        <v>1</v>
-      </c>
-      <c r="E35" s="15">
-        <v>1</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G35" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H35" s="14">
+      <c r="B44" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" s="14">
+        <v>1</v>
+      </c>
+      <c r="D44" s="15">
+        <v>1</v>
+      </c>
+      <c r="E44" s="15">
+        <v>1</v>
+      </c>
+      <c r="F44" s="15">
+        <v>1</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" s="14">
         <v>22</v>
       </c>
-      <c r="I35" s="4"/>
-      <c r="J35" s="14" t="s">
+      <c r="J44" s="4"/>
+      <c r="K44" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="K35" s="14" t="s">
+      <c r="L44" s="14" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A36" s="13" t="s">
+    <row r="45" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A45" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="B36" s="4">
-        <v>0</v>
-      </c>
-      <c r="C36" s="15">
-        <v>1</v>
-      </c>
-      <c r="D36" s="15">
-        <v>1</v>
-      </c>
-      <c r="E36" s="15">
-        <v>1</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H36" s="4">
+      <c r="B45" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="4">
+        <v>0</v>
+      </c>
+      <c r="D45" s="15">
+        <v>1</v>
+      </c>
+      <c r="E45" s="15">
+        <v>1</v>
+      </c>
+      <c r="F45" s="15">
+        <v>1</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I45" s="4">
         <v>21</v>
       </c>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4" t="s">
+      <c r="J45" s="4"/>
+      <c r="K45" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="L45" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A37" s="13" t="s">
+    <row r="46" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A46" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="B37" s="4">
-        <v>0</v>
-      </c>
-      <c r="C37" s="15">
-        <v>1</v>
-      </c>
-      <c r="D37" s="15">
-        <v>1</v>
-      </c>
-      <c r="E37" s="15">
-        <v>1</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H37" s="4">
+      <c r="B46" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="4">
+        <v>0</v>
+      </c>
+      <c r="D46" s="15">
+        <v>1</v>
+      </c>
+      <c r="E46" s="15">
+        <v>1</v>
+      </c>
+      <c r="F46" s="15">
+        <v>1</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I46" s="4">
         <v>23</v>
       </c>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4" t="s">
+      <c r="J46" s="4"/>
+      <c r="K46" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="L46" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A38" s="13" t="s">
+    <row r="47" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A47" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="B38" s="14">
-        <v>0</v>
-      </c>
-      <c r="C38" s="15">
-        <v>1</v>
-      </c>
-      <c r="D38" s="15">
-        <v>1</v>
-      </c>
-      <c r="E38" s="15">
-        <v>1</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" s="14">
+      <c r="B47" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C47" s="14">
+        <v>0</v>
+      </c>
+      <c r="D47" s="15">
+        <v>1</v>
+      </c>
+      <c r="E47" s="15">
+        <v>1</v>
+      </c>
+      <c r="F47" s="15">
+        <v>1</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" s="14">
         <v>21</v>
       </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="14" t="s">
+      <c r="J47" s="4"/>
+      <c r="K47" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="K38" s="14" t="s">
+      <c r="L47" s="14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A39" s="13" t="s">
+    <row r="48" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A48" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="B39" s="4">
-        <v>1</v>
-      </c>
-      <c r="C39" s="15">
-        <v>1</v>
-      </c>
-      <c r="D39" s="15">
-        <v>1</v>
-      </c>
-      <c r="E39" s="15">
-        <v>1</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="4">
+      <c r="B48" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
+      <c r="D48" s="15">
+        <v>1</v>
+      </c>
+      <c r="E48" s="15">
+        <v>1</v>
+      </c>
+      <c r="F48" s="15">
+        <v>1</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="4">
         <v>29</v>
       </c>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4" t="s">
+      <c r="J48" s="4"/>
+      <c r="K48" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="L48" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A40" s="13" t="s">
+    <row r="49" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A49" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="B40" s="4">
-        <v>1</v>
-      </c>
-      <c r="C40" s="15">
-        <v>1</v>
-      </c>
-      <c r="D40" s="15">
-        <v>1</v>
-      </c>
-      <c r="E40" s="15">
-        <v>1</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="4">
+      <c r="B49" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C49" s="4">
+        <v>1</v>
+      </c>
+      <c r="D49" s="15">
+        <v>1</v>
+      </c>
+      <c r="E49" s="15">
+        <v>1</v>
+      </c>
+      <c r="F49" s="15">
+        <v>1</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="4">
         <v>24</v>
       </c>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4" t="s">
+      <c r="J49" s="4"/>
+      <c r="K49" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="K40" s="4" t="s">
+      <c r="L49" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A41" s="13" t="s">
+    <row r="50" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A50" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="B41" s="4">
-        <v>0</v>
-      </c>
-      <c r="C41" s="15">
-        <v>1</v>
-      </c>
-      <c r="D41" s="15">
-        <v>1</v>
-      </c>
-      <c r="E41" s="15">
-        <v>1</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="4">
+      <c r="B50" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C50" s="4">
+        <v>0</v>
+      </c>
+      <c r="D50" s="15">
+        <v>1</v>
+      </c>
+      <c r="E50" s="15">
+        <v>1</v>
+      </c>
+      <c r="F50" s="15">
+        <v>1</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="4">
         <v>30</v>
       </c>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4" t="s">
+      <c r="J50" s="4"/>
+      <c r="K50" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="L50" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A42" s="13" t="s">
+    <row r="51" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A51" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="B42" s="4">
-        <v>1</v>
-      </c>
-      <c r="C42" s="15">
-        <v>1</v>
-      </c>
-      <c r="D42" s="15">
-        <v>1</v>
-      </c>
-      <c r="E42" s="15">
-        <v>1</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" s="4">
+      <c r="B51" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" s="4">
+        <v>1</v>
+      </c>
+      <c r="D51" s="15">
+        <v>1</v>
+      </c>
+      <c r="E51" s="15">
+        <v>1</v>
+      </c>
+      <c r="F51" s="15">
+        <v>1</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="4">
         <v>29</v>
       </c>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4" t="s">
+      <c r="J51" s="4"/>
+      <c r="K51" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="K42" s="4" t="s">
+      <c r="L51" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A43" s="13" t="s">
+    <row r="52" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A52" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="B43" s="4">
-        <v>1</v>
-      </c>
-      <c r="C43" s="15">
-        <v>1</v>
-      </c>
-      <c r="D43" s="15">
-        <v>1</v>
-      </c>
-      <c r="E43" s="15">
-        <v>1</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H43" s="4">
+      <c r="B52" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" s="4">
+        <v>1</v>
+      </c>
+      <c r="D52" s="15">
+        <v>1</v>
+      </c>
+      <c r="E52" s="15">
+        <v>1</v>
+      </c>
+      <c r="F52" s="15">
+        <v>1</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" s="4">
         <v>23</v>
       </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4" t="s">
+      <c r="J52" s="4"/>
+      <c r="K52" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="L52" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A44" s="13" t="s">
+    <row r="53" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A53" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="B44" s="4">
-        <v>1</v>
-      </c>
-      <c r="C44" s="15">
-        <v>1</v>
-      </c>
-      <c r="D44" s="15">
-        <v>1</v>
-      </c>
-      <c r="E44" s="15">
-        <v>1</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" s="4">
+      <c r="B53" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C53" s="4">
+        <v>1</v>
+      </c>
+      <c r="D53" s="15">
+        <v>1</v>
+      </c>
+      <c r="E53" s="15">
+        <v>1</v>
+      </c>
+      <c r="F53" s="15">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I53" s="4">
         <v>34</v>
       </c>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4" t="s">
+      <c r="J53" s="4"/>
+      <c r="K53" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="K44" s="4" t="s">
+      <c r="L53" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A45" s="13" t="s">
+    <row r="54" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A54" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="E54" s="15">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I54" s="4">
+        <v>22</v>
+      </c>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A55" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="B45" s="4">
-        <v>1</v>
-      </c>
-      <c r="C45" s="15">
-        <v>1</v>
-      </c>
-      <c r="D45" s="15">
-        <v>1</v>
-      </c>
-      <c r="E45" s="15">
-        <v>1</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" s="4">
+      <c r="B55" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" s="4">
+        <v>1</v>
+      </c>
+      <c r="D55" s="15">
+        <v>1</v>
+      </c>
+      <c r="E55" s="15">
+        <v>1</v>
+      </c>
+      <c r="F55" s="15">
+        <v>1</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" s="4">
         <v>22</v>
       </c>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4" t="s">
+      <c r="J55" s="4"/>
+      <c r="K55" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="L55" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A46" s="13" t="s">
+    <row r="56" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A56" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="B46" s="4">
-        <v>1</v>
-      </c>
-      <c r="C46" s="15">
-        <v>1</v>
-      </c>
-      <c r="D46" s="15">
-        <v>1</v>
-      </c>
-      <c r="E46" s="15">
-        <v>1</v>
-      </c>
-      <c r="F46" s="4" t="s">
+      <c r="B56" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="C56" s="4">
+        <v>1</v>
+      </c>
+      <c r="D56" s="15">
+        <v>1</v>
+      </c>
+      <c r="E56" s="15">
+        <v>1</v>
+      </c>
+      <c r="F56" s="15">
+        <v>1</v>
+      </c>
+      <c r="G56" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="4">
+      <c r="H56" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I56" s="4">
         <v>18</v>
       </c>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4" t="s">
+      <c r="J56" s="4"/>
+      <c r="K56" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="K46" s="4" t="s">
+      <c r="L56" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A47" s="13" t="s">
+    <row r="57" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A57" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="B47" s="4">
-        <v>1</v>
-      </c>
-      <c r="C47" s="15">
-        <v>1</v>
-      </c>
-      <c r="D47" s="15">
-        <v>1</v>
-      </c>
-      <c r="E47" s="15">
-        <v>1</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H47" s="4">
+      <c r="B57" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="C57" s="4">
+        <v>1</v>
+      </c>
+      <c r="D57" s="15">
+        <v>1</v>
+      </c>
+      <c r="E57" s="15">
+        <v>1</v>
+      </c>
+      <c r="F57" s="15">
+        <v>1</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I57" s="4">
         <v>22</v>
       </c>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4" t="s">
+      <c r="J57" s="4"/>
+      <c r="K57" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="K47" s="4" t="s">
+      <c r="L57" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A48" s="13" t="s">
+    <row r="58" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A58" s="34" t="s">
         <v>187</v>
       </c>
-      <c r="B48" s="4">
-        <v>0</v>
-      </c>
-      <c r="C48" s="15">
-        <v>1</v>
-      </c>
-      <c r="D48" s="15">
-        <v>1</v>
-      </c>
-      <c r="E48" s="15">
-        <v>1</v>
-      </c>
-      <c r="F48" s="4" t="s">
+      <c r="B58" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0</v>
+      </c>
+      <c r="D58" s="15">
+        <v>1</v>
+      </c>
+      <c r="E58" s="15">
+        <v>1</v>
+      </c>
+      <c r="F58" s="15">
+        <v>1</v>
+      </c>
+      <c r="G58" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="G48" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H48" s="4">
+      <c r="H58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I58" s="4">
         <v>22</v>
       </c>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4" t="s">
+      <c r="J58" s="4"/>
+      <c r="K58" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="L58" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A49" s="13" t="s">
+    <row r="59" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A59" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="B49" s="4">
-        <v>1</v>
-      </c>
-      <c r="C49" s="15">
-        <v>1</v>
-      </c>
-      <c r="D49" s="15">
-        <v>1</v>
-      </c>
-      <c r="E49" s="15">
-        <v>1</v>
-      </c>
-      <c r="F49" s="4" t="s">
+      <c r="B59" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C59" s="4">
+        <v>1</v>
+      </c>
+      <c r="D59" s="15">
+        <v>1</v>
+      </c>
+      <c r="E59" s="15">
+        <v>1</v>
+      </c>
+      <c r="F59" s="15">
+        <v>1</v>
+      </c>
+      <c r="G59" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="G49" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H49" s="4">
+      <c r="H59" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I59" s="4">
         <v>20</v>
       </c>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4" t="s">
+      <c r="J59" s="4"/>
+      <c r="K59" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="K49" s="4" t="s">
+      <c r="L59" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A50" s="13" t="s">
+    <row r="60" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="A60" s="34" t="s">
         <v>191</v>
       </c>
-      <c r="B50" s="4">
-        <v>1</v>
-      </c>
-      <c r="C50" s="15">
-        <v>1</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="4">
+      <c r="B60" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="C60" s="4">
+        <v>1</v>
+      </c>
+      <c r="D60" s="15">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I60" s="4">
         <v>22</v>
       </c>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4" t="s">
+      <c r="J60" s="4"/>
+      <c r="K60" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="K50" s="4" t="s">
+      <c r="L60" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="I51" s="4"/>
-    </row>
-    <row r="52" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="I52" s="4"/>
-    </row>
-    <row r="53" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="B53" s="4">
-        <f>SUM(B1:B50)</f>
+    <row r="64" spans="1:12" ht="17.100000000000001" customHeight="1">
+      <c r="J64" s="4"/>
+    </row>
+    <row r="65" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A65" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="J65" s="4"/>
+    </row>
+    <row r="66" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A66" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66" s="4">
+        <f>SUM(C2:C62)</f>
+        <v>40</v>
+      </c>
+      <c r="J66" s="4"/>
+    </row>
+    <row r="67" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A67" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="J67" s="4"/>
+    </row>
+    <row r="68" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A68" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="J68" s="4"/>
+    </row>
+    <row r="69" spans="1:10" ht="17.100000000000001" customHeight="1">
+      <c r="A69" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="J69" s="4"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="J70" s="4"/>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="J71" s="4"/>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="J72" s="4"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="J73" s="4"/>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="J74" s="4"/>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="J75" s="4"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="I53" s="4"/>
-    </row>
-    <row r="54" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="I54" s="4"/>
-    </row>
-    <row r="55" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="I55" s="4"/>
-    </row>
-    <row r="56" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="I56" s="4"/>
-    </row>
-    <row r="57" spans="1:11">
-      <c r="I57" s="4"/>
-    </row>
-    <row r="58" spans="1:11">
-      <c r="I58" s="4"/>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="I59" s="4"/>
-    </row>
-    <row r="60" spans="1:11">
-      <c r="I60" s="4"/>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="I61" s="4"/>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="I62" s="4"/>
-    </row>
-    <row r="63" spans="1:11">
-      <c r="I63" s="4"/>
-    </row>
-    <row r="64" spans="1:11">
-      <c r="I64" s="4"/>
-    </row>
-    <row r="65" spans="9:9">
-      <c r="I65" s="4"/>
-    </row>
-    <row r="66" spans="9:9">
-      <c r="I66" s="4"/>
-    </row>
-    <row r="67" spans="9:9">
-      <c r="I67" s="4"/>
-    </row>
-    <row r="68" spans="9:9">
-      <c r="I68" s="4"/>
-    </row>
-    <row r="69" spans="9:9">
-      <c r="I69" s="4"/>
-    </row>
-    <row r="70" spans="9:9">
-      <c r="I70" s="4"/>
-    </row>
-    <row r="71" spans="9:9">
-      <c r="I71" s="4"/>
-    </row>
-    <row r="72" spans="9:9">
-      <c r="I72" s="4"/>
-    </row>
-    <row r="73" spans="9:9">
-      <c r="I73" s="4"/>
-    </row>
-    <row r="74" spans="9:9">
-      <c r="I74" s="4"/>
-    </row>
-    <row r="75" spans="9:9">
-      <c r="I75" s="4"/>
-    </row>
-    <row r="76" spans="9:9">
-      <c r="I76" s="4"/>
-    </row>
-    <row r="77" spans="9:9">
-      <c r="I77" s="4"/>
-    </row>
-    <row r="78" spans="9:9">
-      <c r="I78" s="4"/>
-    </row>
-    <row r="79" spans="9:9">
-      <c r="I79" s="4"/>
-    </row>
-    <row r="80" spans="9:9">
-      <c r="I80" s="4"/>
-    </row>
-    <row r="81" spans="9:9">
-      <c r="I81" s="4"/>
-    </row>
-    <row r="82" spans="9:9">
-      <c r="I82" s="4"/>
-    </row>
-    <row r="83" spans="9:9">
-      <c r="I83" s="4"/>
-    </row>
-    <row r="84" spans="9:9">
-      <c r="I84" s="4"/>
-    </row>
-    <row r="85" spans="9:9">
-      <c r="I85" s="4"/>
-    </row>
-    <row r="86" spans="9:9">
-      <c r="I86" s="4"/>
-    </row>
-    <row r="87" spans="9:9">
-      <c r="I87" s="4"/>
-    </row>
-    <row r="88" spans="9:9">
-      <c r="I88" s="4"/>
-    </row>
-    <row r="89" spans="9:9">
-      <c r="I89" s="4"/>
-    </row>
-    <row r="90" spans="9:9">
-      <c r="I90" s="4"/>
-    </row>
-    <row r="91" spans="9:9">
-      <c r="I91" s="4"/>
-    </row>
-    <row r="92" spans="9:9">
-      <c r="I92" s="4"/>
-    </row>
-    <row r="93" spans="9:9">
-      <c r="I93" s="4"/>
-    </row>
-    <row r="94" spans="9:9">
-      <c r="I94" s="4"/>
-    </row>
-    <row r="95" spans="9:9">
-      <c r="I95" s="4"/>
-    </row>
-    <row r="96" spans="9:9">
-      <c r="I96" s="4"/>
-    </row>
-    <row r="97" spans="9:9">
-      <c r="I97" s="4"/>
-    </row>
-    <row r="98" spans="9:9">
-      <c r="I98" s="4"/>
-    </row>
-    <row r="99" spans="9:9">
-      <c r="I99" s="4"/>
-    </row>
-    <row r="100" spans="9:9">
-      <c r="I100" s="4"/>
-    </row>
-    <row r="101" spans="9:9">
-      <c r="I101" s="4"/>
-    </row>
-    <row r="102" spans="9:9">
-      <c r="I102" s="4"/>
-    </row>
-    <row r="103" spans="9:9">
-      <c r="I103" s="4"/>
-    </row>
-    <row r="104" spans="9:9">
-      <c r="I104" s="4"/>
-    </row>
-    <row r="105" spans="9:9">
-      <c r="I105" s="4"/>
-    </row>
-    <row r="106" spans="9:9">
-      <c r="I106" s="4"/>
-    </row>
-    <row r="107" spans="9:9">
-      <c r="I107" s="4"/>
-    </row>
-    <row r="108" spans="9:9">
-      <c r="I108" s="4"/>
-    </row>
-    <row r="109" spans="9:9">
-      <c r="I109" s="4"/>
-    </row>
-    <row r="110" spans="9:9">
-      <c r="I110" s="4"/>
-    </row>
-    <row r="111" spans="9:9">
-      <c r="I111" s="4"/>
-    </row>
-    <row r="112" spans="9:9">
-      <c r="I112" s="4"/>
-    </row>
-    <row r="113" spans="9:9">
-      <c r="I113" s="4"/>
-    </row>
-    <row r="114" spans="9:9">
-      <c r="I114" s="4"/>
-    </row>
-    <row r="115" spans="9:9">
-      <c r="I115" s="4"/>
-    </row>
-    <row r="116" spans="9:9">
-      <c r="I116" s="4"/>
-    </row>
-    <row r="117" spans="9:9">
-      <c r="I117" s="4"/>
+      <c r="J76" s="4"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="J77" s="4"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="J78" s="4"/>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="J79" s="4"/>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="J80" s="4"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="J81" s="4"/>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="J82" s="4"/>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="J83" s="4"/>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="J84" s="4"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="J85" s="4"/>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="J86" s="4"/>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="J87" s="4"/>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="J88" s="4"/>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="J89" s="4"/>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="J90" s="4"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="J91" s="4"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="J92" s="4"/>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="J93" s="4"/>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="J94" s="4"/>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="J95" s="4"/>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="J96" s="4"/>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="J97" s="4"/>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="J98" s="4"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="J99" s="4"/>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="J100" s="4"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="J101" s="4"/>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="J102" s="4"/>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="J103" s="4"/>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="J104" s="4"/>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="J105" s="4"/>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="J106" s="4"/>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="J107" s="4"/>
+    </row>
+    <row r="108" spans="1:10">
+      <c r="A108" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="J108" s="4"/>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="J109" s="4"/>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="J110" s="4"/>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="J111" s="4"/>
+    </row>
+    <row r="112" spans="1:10">
+      <c r="A112" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="J112" s="4"/>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="J113" s="4"/>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="J114" s="4"/>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="J115" s="4"/>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="J116" s="4"/>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="J117" s="4"/>
+    </row>
+    <row r="118" spans="1:10">
+      <c r="A118" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="J118" s="4"/>
+    </row>
+    <row r="119" spans="1:10">
+      <c r="A119" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="J119" s="4"/>
+    </row>
+    <row r="120" spans="1:10">
+      <c r="A120" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="J120" s="4"/>
+    </row>
+    <row r="121" spans="1:10">
+      <c r="A121" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="J121" s="4"/>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="J122" s="4"/>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="J123" s="4"/>
+    </row>
+    <row r="124" spans="1:10">
+      <c r="A124" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="J124" s="4"/>
+    </row>
+    <row r="125" spans="1:10">
+      <c r="A125" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="J125" s="4"/>
+    </row>
+    <row r="126" spans="1:10">
+      <c r="A126" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="J126" s="4"/>
+    </row>
+    <row r="127" spans="1:10">
+      <c r="J127" s="4"/>
+    </row>
+    <row r="128" spans="1:10">
+      <c r="J128" s="4"/>
+    </row>
+    <row r="129" spans="10:10">
+      <c r="J129" s="4"/>
+    </row>
+    <row r="130" spans="10:10">
+      <c r="J130" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A1:K128">
-    <sortCondition ref="A1:A128"/>
+  <sortState ref="C1:M128">
+    <sortCondition ref="C1:C128"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Results Table MRI Results (Added RT Analysis)
</commit_message>
<xml_diff>
--- a/data/Demographics.xlsx
+++ b/data/Demographics.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11475" yWindow="1200" windowWidth="28245" windowHeight="17235"/>
+    <workbookView xWindow="11475" yWindow="1200" windowWidth="28245" windowHeight="17235" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
     <sheet name="MDD" sheetId="4" r:id="rId2"/>
     <sheet name="RT Analysis" sheetId="5" r:id="rId3"/>
-    <sheet name="EEG Analysis" sheetId="3" r:id="rId4"/>
-    <sheet name="fMRI Analysis" sheetId="6" r:id="rId5"/>
+    <sheet name="MDD_EEG Analysis" sheetId="3" r:id="rId4"/>
+    <sheet name="MDD_fMRI Analysis" sheetId="6" r:id="rId5"/>
+    <sheet name="fMRT_RT_Analysis" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="242">
   <si>
     <t>Healthy Control (HC) or Patient</t>
   </si>
@@ -1106,7 +1107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1212,6 +1213,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1534,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J74" sqref="J74:J75"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15.75"/>
@@ -12406,4 +12410,3465 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J115"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" activeCellId="4" sqref="A1:A1048576 E1:E1048576 F1:F1048576 G1:G1048576 H1:H1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="14" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="16" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="53.125" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="9.125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="19" customFormat="1" ht="30">
+      <c r="A1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="15">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15">
+        <v>1</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1</v>
+      </c>
+      <c r="D3" s="15">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2">
+        <v>23</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="60">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="15">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="2">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="15">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="15">
+        <v>1</v>
+      </c>
+      <c r="C6" s="15">
+        <v>1</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="2">
+        <v>27</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="15">
+        <v>1</v>
+      </c>
+      <c r="C7" s="15">
+        <v>1</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2">
+        <v>22</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="15">
+        <v>1</v>
+      </c>
+      <c r="C8" s="15">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2">
+        <v>18</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="60">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="15">
+        <v>1</v>
+      </c>
+      <c r="C9" s="15">
+        <v>1</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2">
+        <v>36</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="15">
+        <v>1</v>
+      </c>
+      <c r="C10" s="15">
+        <v>1</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="2">
+        <v>26</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="15">
+        <v>1</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2">
+        <v>28</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="15">
+        <v>1</v>
+      </c>
+      <c r="C12" s="15">
+        <v>1</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="2">
+        <v>26</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="15">
+        <v>1</v>
+      </c>
+      <c r="C13" s="15">
+        <v>1</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2">
+        <v>22</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="15">
+        <v>1</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1</v>
+      </c>
+      <c r="D14" s="15">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="2">
+        <v>22</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="2">
+        <v>23</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="15">
+        <v>1</v>
+      </c>
+      <c r="C16" s="15">
+        <v>1</v>
+      </c>
+      <c r="D16" s="15">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="2">
+        <v>25</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="15">
+        <v>1</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1</v>
+      </c>
+      <c r="D17" s="15">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2">
+        <v>23</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="15">
+        <v>1</v>
+      </c>
+      <c r="C18" s="15">
+        <v>1</v>
+      </c>
+      <c r="D18" s="15">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="2">
+        <v>32</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="45">
+      <c r="A19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="15">
+        <v>1</v>
+      </c>
+      <c r="C19" s="15">
+        <v>1</v>
+      </c>
+      <c r="D19" s="15">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="2">
+        <v>26</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="15">
+        <v>1</v>
+      </c>
+      <c r="C20" s="15">
+        <v>1</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="2">
+        <v>22</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="15">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="2">
+        <v>26</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="15">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="2">
+        <v>21</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="15">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="2">
+        <v>26</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="15">
+        <v>1</v>
+      </c>
+      <c r="C24" s="15">
+        <v>1</v>
+      </c>
+      <c r="D24" s="15">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="2">
+        <v>21</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="15">
+        <v>1</v>
+      </c>
+      <c r="C25" s="15">
+        <v>1</v>
+      </c>
+      <c r="D25" s="15">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="2">
+        <v>25</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="15">
+        <v>1</v>
+      </c>
+      <c r="C26" s="15">
+        <v>1</v>
+      </c>
+      <c r="D26" s="15">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="2">
+        <v>33</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="15">
+        <v>1</v>
+      </c>
+      <c r="C27" s="15">
+        <v>1</v>
+      </c>
+      <c r="D27" s="15">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="2">
+        <v>25</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" ht="60">
+      <c r="A28" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="15">
+        <v>1</v>
+      </c>
+      <c r="C28" s="15">
+        <v>1</v>
+      </c>
+      <c r="D28" s="15">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="2">
+        <v>30</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="60">
+      <c r="A29" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="15">
+        <v>1</v>
+      </c>
+      <c r="C29" s="15">
+        <v>1</v>
+      </c>
+      <c r="D29" s="15">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="2">
+        <v>18</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45">
+      <c r="A30" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="15">
+        <v>1</v>
+      </c>
+      <c r="C30" s="15">
+        <v>1</v>
+      </c>
+      <c r="D30" s="15">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="2">
+        <v>30</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="60">
+      <c r="A31" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="15">
+        <v>1</v>
+      </c>
+      <c r="C31" s="15">
+        <v>1</v>
+      </c>
+      <c r="D31" s="15">
+        <v>1</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="2">
+        <v>38</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="15">
+        <v>1</v>
+      </c>
+      <c r="C32" s="15">
+        <v>1</v>
+      </c>
+      <c r="D32" s="15">
+        <v>1</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="2">
+        <v>21</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="60">
+      <c r="A33" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="15">
+        <v>1</v>
+      </c>
+      <c r="C33" s="15">
+        <v>1</v>
+      </c>
+      <c r="D33" s="15">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="2">
+        <v>27</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="15">
+        <v>1</v>
+      </c>
+      <c r="C34" s="15">
+        <v>1</v>
+      </c>
+      <c r="D34" s="15">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="2">
+        <v>23</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="15">
+        <v>1</v>
+      </c>
+      <c r="C35" s="15">
+        <v>1</v>
+      </c>
+      <c r="D35" s="15">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="2">
+        <v>44</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="15">
+        <v>1</v>
+      </c>
+      <c r="C36" s="15">
+        <v>1</v>
+      </c>
+      <c r="D36" s="15">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="2">
+        <v>36</v>
+      </c>
+      <c r="H36" s="2">
+        <v>1</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="15">
+        <v>1</v>
+      </c>
+      <c r="C37" s="15">
+        <v>1</v>
+      </c>
+      <c r="D37" s="15">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="2">
+        <v>22</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="15">
+        <v>1</v>
+      </c>
+      <c r="C38" s="15">
+        <v>1</v>
+      </c>
+      <c r="D38" s="15">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="2">
+        <v>30</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+      <c r="I38" s="2"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="15">
+        <v>1</v>
+      </c>
+      <c r="C39" s="15">
+        <v>1</v>
+      </c>
+      <c r="D39" s="15">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" s="2">
+        <v>21</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" ht="60">
+      <c r="A40" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
+      <c r="C40" s="15">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G40" s="2">
+        <v>21</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="60">
+      <c r="A41" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="15">
+        <v>1</v>
+      </c>
+      <c r="C41" s="15">
+        <v>1</v>
+      </c>
+      <c r="D41" s="15">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="2">
+        <v>28</v>
+      </c>
+      <c r="H41" s="2">
+        <v>1</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0</v>
+      </c>
+      <c r="C42" s="15">
+        <v>1</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="2">
+        <v>21</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="15">
+        <v>1</v>
+      </c>
+      <c r="C43" s="15">
+        <v>1</v>
+      </c>
+      <c r="D43" s="15">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="2">
+        <v>27</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="15">
+        <v>1</v>
+      </c>
+      <c r="C44" s="15">
+        <v>1</v>
+      </c>
+      <c r="D44" s="15">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="2">
+        <v>33</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="15">
+        <v>1</v>
+      </c>
+      <c r="C45" s="15">
+        <v>1</v>
+      </c>
+      <c r="D45" s="15">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="2">
+        <v>36</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0</v>
+      </c>
+      <c r="I45" s="2"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="15">
+        <v>1</v>
+      </c>
+      <c r="C46" s="15">
+        <v>1</v>
+      </c>
+      <c r="D46" s="15">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="2">
+        <v>23</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="3">
+        <v>0</v>
+      </c>
+      <c r="C47" s="15">
+        <v>1</v>
+      </c>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="2">
+        <v>22</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0</v>
+      </c>
+      <c r="I47" s="2"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B48" s="15">
+        <v>1</v>
+      </c>
+      <c r="C48" s="15">
+        <v>1</v>
+      </c>
+      <c r="D48" s="15">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="2">
+        <v>24</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" s="15">
+        <v>1</v>
+      </c>
+      <c r="C49" s="15">
+        <v>1</v>
+      </c>
+      <c r="D49" s="15">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="2">
+        <v>25</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0</v>
+      </c>
+      <c r="I49" s="2"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="15">
+        <v>1</v>
+      </c>
+      <c r="C50" s="15">
+        <v>1</v>
+      </c>
+      <c r="D50" s="15">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="2">
+        <v>25</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0</v>
+      </c>
+      <c r="I50" s="2"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51" s="15">
+        <v>1</v>
+      </c>
+      <c r="C51" s="15">
+        <v>1</v>
+      </c>
+      <c r="D51" s="15">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="2">
+        <v>24</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0</v>
+      </c>
+      <c r="I51" s="2"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="15">
+        <v>1</v>
+      </c>
+      <c r="C52" s="15">
+        <v>1</v>
+      </c>
+      <c r="D52" s="15">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="2">
+        <v>22</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="45">
+      <c r="A53" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="15">
+        <v>1</v>
+      </c>
+      <c r="C53" s="15">
+        <v>1</v>
+      </c>
+      <c r="D53" s="15">
+        <v>1</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" s="2">
+        <v>26</v>
+      </c>
+      <c r="H53" s="2">
+        <v>1</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="60">
+      <c r="A54" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="15">
+        <v>1</v>
+      </c>
+      <c r="C54" s="15">
+        <v>1</v>
+      </c>
+      <c r="D54" s="15">
+        <v>1</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" s="2">
+        <v>18</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="30">
+      <c r="A55" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55" s="3">
+        <v>0</v>
+      </c>
+      <c r="C55" s="15">
+        <v>1</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="2">
+        <v>37</v>
+      </c>
+      <c r="H55" s="2">
+        <v>1</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="15">
+        <v>1</v>
+      </c>
+      <c r="C56" s="15">
+        <v>1</v>
+      </c>
+      <c r="D56" s="15">
+        <v>1</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="2">
+        <v>24</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0</v>
+      </c>
+      <c r="I56" s="2"/>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="15">
+        <v>1</v>
+      </c>
+      <c r="C57" s="15">
+        <v>1</v>
+      </c>
+      <c r="D57" s="15">
+        <v>1</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="2">
+        <v>35</v>
+      </c>
+      <c r="H57" s="2">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2"/>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="15">
+        <v>1</v>
+      </c>
+      <c r="C58" s="15">
+        <v>1</v>
+      </c>
+      <c r="D58" s="15">
+        <v>1</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" s="2">
+        <v>19</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="15">
+        <v>1</v>
+      </c>
+      <c r="C59" s="15">
+        <v>1</v>
+      </c>
+      <c r="D59" s="15">
+        <v>1</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="2">
+        <v>26</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0</v>
+      </c>
+      <c r="I59" s="2"/>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="1:10" ht="30">
+      <c r="A60" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" s="15">
+        <v>1</v>
+      </c>
+      <c r="C60" s="15">
+        <v>1</v>
+      </c>
+      <c r="D60" s="15">
+        <v>1</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" s="2">
+        <v>18</v>
+      </c>
+      <c r="H60" s="2">
+        <v>1</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" s="15">
+        <v>1</v>
+      </c>
+      <c r="C61" s="15">
+        <v>1</v>
+      </c>
+      <c r="D61" s="15">
+        <v>1</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="2">
+        <v>22</v>
+      </c>
+      <c r="H61" s="2">
+        <v>0</v>
+      </c>
+      <c r="I61" s="2"/>
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B62" s="15">
+        <v>1</v>
+      </c>
+      <c r="C62" s="15">
+        <v>1</v>
+      </c>
+      <c r="D62" s="15">
+        <v>1</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G62" s="2">
+        <v>41</v>
+      </c>
+      <c r="H62" s="2">
+        <v>0</v>
+      </c>
+      <c r="I62" s="2"/>
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="1:10" ht="45">
+      <c r="A63" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" s="15">
+        <v>1</v>
+      </c>
+      <c r="C63" s="15">
+        <v>1</v>
+      </c>
+      <c r="D63" s="15">
+        <v>1</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63" s="2">
+        <v>39</v>
+      </c>
+      <c r="H63" s="2">
+        <v>1</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="30">
+      <c r="A64" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" s="15">
+        <v>1</v>
+      </c>
+      <c r="C64" s="15">
+        <v>1</v>
+      </c>
+      <c r="D64" s="15">
+        <v>1</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" s="2">
+        <v>22</v>
+      </c>
+      <c r="H64" s="2">
+        <v>0</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" s="15">
+        <v>1</v>
+      </c>
+      <c r="C65" s="15">
+        <v>1</v>
+      </c>
+      <c r="D65" s="15">
+        <v>1</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="2">
+        <v>23</v>
+      </c>
+      <c r="H65" s="2">
+        <v>0</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" s="15">
+        <v>1</v>
+      </c>
+      <c r="C66" s="15">
+        <v>1</v>
+      </c>
+      <c r="D66" s="15">
+        <v>1</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" s="2">
+        <v>21</v>
+      </c>
+      <c r="H66" s="2">
+        <v>0</v>
+      </c>
+      <c r="I66" s="2"/>
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" s="3">
+        <v>0</v>
+      </c>
+      <c r="C67" s="15">
+        <v>1</v>
+      </c>
+      <c r="D67" s="3">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" s="2">
+        <v>24</v>
+      </c>
+      <c r="H67" s="2">
+        <v>0</v>
+      </c>
+      <c r="I67" s="2"/>
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="1:10" ht="105">
+      <c r="A68" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" s="15">
+        <v>1</v>
+      </c>
+      <c r="C68" s="15">
+        <v>1</v>
+      </c>
+      <c r="D68" s="15">
+        <v>1</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G68" s="2">
+        <v>32</v>
+      </c>
+      <c r="H68" s="2">
+        <v>1</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="30">
+      <c r="A69" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B69" s="15">
+        <v>1</v>
+      </c>
+      <c r="C69" s="15">
+        <v>1</v>
+      </c>
+      <c r="D69" s="15">
+        <v>1</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69" s="2">
+        <v>27</v>
+      </c>
+      <c r="H69" s="2">
+        <v>1</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" s="15">
+        <v>1</v>
+      </c>
+      <c r="C70" s="15">
+        <v>1</v>
+      </c>
+      <c r="D70" s="15">
+        <v>1</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G70" s="2">
+        <v>24</v>
+      </c>
+      <c r="H70" s="2">
+        <v>0</v>
+      </c>
+      <c r="I70" s="2"/>
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="1:10" ht="45">
+      <c r="A71" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B71" s="15">
+        <v>1</v>
+      </c>
+      <c r="C71" s="15">
+        <v>1</v>
+      </c>
+      <c r="D71" s="15">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" s="2">
+        <v>20</v>
+      </c>
+      <c r="H71" s="2">
+        <v>1</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" s="15">
+        <v>1</v>
+      </c>
+      <c r="C72" s="15">
+        <v>1</v>
+      </c>
+      <c r="D72" s="15">
+        <v>1</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G72" s="2">
+        <v>21</v>
+      </c>
+      <c r="H72" s="2">
+        <v>0</v>
+      </c>
+      <c r="I72" s="2"/>
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" s="15">
+        <v>1</v>
+      </c>
+      <c r="C73" s="15">
+        <v>1</v>
+      </c>
+      <c r="D73" s="15">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73" s="2">
+        <v>22</v>
+      </c>
+      <c r="H73" s="2">
+        <v>0</v>
+      </c>
+      <c r="I73" s="2"/>
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="1:10" ht="60">
+      <c r="A74" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" s="3">
+        <v>0</v>
+      </c>
+      <c r="C74" s="15">
+        <v>1</v>
+      </c>
+      <c r="D74" s="3">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" s="2">
+        <v>21</v>
+      </c>
+      <c r="H74" s="2">
+        <v>1</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" s="15">
+        <v>1</v>
+      </c>
+      <c r="C75" s="15">
+        <v>1</v>
+      </c>
+      <c r="D75" s="15">
+        <v>1</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G75" s="2">
+        <v>27</v>
+      </c>
+      <c r="H75" s="2">
+        <v>0</v>
+      </c>
+      <c r="I75" s="2"/>
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" s="15">
+        <v>1</v>
+      </c>
+      <c r="C76" s="15">
+        <v>1</v>
+      </c>
+      <c r="D76" s="15">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" s="2">
+        <v>52</v>
+      </c>
+      <c r="H76" s="2">
+        <v>0</v>
+      </c>
+      <c r="I76" s="2"/>
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" s="15">
+        <v>1</v>
+      </c>
+      <c r="C77" s="15">
+        <v>1</v>
+      </c>
+      <c r="D77" s="15">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G77" s="2">
+        <v>35</v>
+      </c>
+      <c r="H77" s="2">
+        <v>0</v>
+      </c>
+      <c r="I77" s="2"/>
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" s="15">
+        <v>1</v>
+      </c>
+      <c r="C78" s="15">
+        <v>1</v>
+      </c>
+      <c r="D78" s="15">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G78" s="2">
+        <v>30</v>
+      </c>
+      <c r="H78" s="2">
+        <v>0</v>
+      </c>
+      <c r="I78" s="2"/>
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="1:10" ht="47.25">
+      <c r="A79" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B79" s="3">
+        <v>0</v>
+      </c>
+      <c r="C79" s="15">
+        <v>1</v>
+      </c>
+      <c r="D79" s="3">
+        <v>0</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G79" s="2">
+        <v>22</v>
+      </c>
+      <c r="H79" s="2">
+        <v>1</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="15">
+        <v>1</v>
+      </c>
+      <c r="C80" s="15">
+        <v>1</v>
+      </c>
+      <c r="D80" s="15">
+        <v>1</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G80" s="2">
+        <v>19</v>
+      </c>
+      <c r="H80" s="2">
+        <v>0</v>
+      </c>
+      <c r="I80" s="2"/>
+    </row>
+    <row r="81" spans="1:10" ht="31.5">
+      <c r="A81" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" s="3">
+        <v>0</v>
+      </c>
+      <c r="C81" s="15">
+        <v>1</v>
+      </c>
+      <c r="D81" s="3">
+        <v>0</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" s="2">
+        <v>25</v>
+      </c>
+      <c r="H81" s="2">
+        <v>1</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" s="15">
+        <v>1</v>
+      </c>
+      <c r="C82" s="15">
+        <v>1</v>
+      </c>
+      <c r="D82" s="15">
+        <v>1</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G82" s="2">
+        <v>23</v>
+      </c>
+      <c r="H82" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="45">
+      <c r="A83" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B83" s="15">
+        <v>1</v>
+      </c>
+      <c r="C83" s="15">
+        <v>1</v>
+      </c>
+      <c r="D83" s="15">
+        <v>1</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G83" s="2">
+        <v>22</v>
+      </c>
+      <c r="H83" s="2">
+        <v>1</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="J83" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="16.5" customHeight="1">
+      <c r="A84" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B84" s="15">
+        <v>1</v>
+      </c>
+      <c r="C84" s="15">
+        <v>1</v>
+      </c>
+      <c r="D84" s="15">
+        <v>1</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G84" s="2">
+        <v>25</v>
+      </c>
+      <c r="H84" s="2">
+        <v>0</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J84" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="30">
+      <c r="A85" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B85" s="15">
+        <v>1</v>
+      </c>
+      <c r="C85" s="15">
+        <v>1</v>
+      </c>
+      <c r="D85" s="15">
+        <v>1</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G85" s="2">
+        <v>31</v>
+      </c>
+      <c r="H85" s="2">
+        <v>0</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J85" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="47.25">
+      <c r="A86" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B86" s="15">
+        <v>1</v>
+      </c>
+      <c r="C86" s="15">
+        <v>1</v>
+      </c>
+      <c r="D86" s="15">
+        <v>1</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G86" s="2">
+        <v>27</v>
+      </c>
+      <c r="H86" s="2">
+        <v>0</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="110.25">
+      <c r="A87" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B87" s="15">
+        <v>1</v>
+      </c>
+      <c r="C87" s="15">
+        <v>1</v>
+      </c>
+      <c r="D87" s="15">
+        <v>1</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G87" s="2">
+        <v>22</v>
+      </c>
+      <c r="H87" s="2">
+        <v>1</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="J87" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B88" s="15">
+        <v>1</v>
+      </c>
+      <c r="C88" s="15">
+        <v>1</v>
+      </c>
+      <c r="D88" s="15">
+        <v>1</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88" s="2">
+        <v>43</v>
+      </c>
+      <c r="H88" s="2">
+        <v>0</v>
+      </c>
+      <c r="I88" s="2"/>
+    </row>
+    <row r="89" spans="1:10" ht="94.5">
+      <c r="A89" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B89" s="15">
+        <v>1</v>
+      </c>
+      <c r="C89" s="15">
+        <v>1</v>
+      </c>
+      <c r="D89" s="15">
+        <v>1</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G89" s="2">
+        <v>28</v>
+      </c>
+      <c r="H89" s="2">
+        <v>0</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="78.75">
+      <c r="A90" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B90" s="15">
+        <v>1</v>
+      </c>
+      <c r="C90" s="15">
+        <v>1</v>
+      </c>
+      <c r="D90" s="15">
+        <v>1</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G90" s="4">
+        <v>21</v>
+      </c>
+      <c r="H90" s="4">
+        <v>1</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="78.75">
+      <c r="A91" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B91" s="15">
+        <v>1</v>
+      </c>
+      <c r="C91" s="15">
+        <v>1</v>
+      </c>
+      <c r="D91" s="15">
+        <v>1</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="4">
+        <v>34</v>
+      </c>
+      <c r="H91" s="4">
+        <v>1</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="J91" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="63">
+      <c r="A92" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B92" s="15">
+        <v>1</v>
+      </c>
+      <c r="C92" s="15">
+        <v>1</v>
+      </c>
+      <c r="D92" s="15">
+        <v>1</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G92" s="4">
+        <v>26</v>
+      </c>
+      <c r="H92" s="4">
+        <v>2</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="60">
+      <c r="A93" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B93" s="15">
+        <v>1</v>
+      </c>
+      <c r="C93" s="15">
+        <v>1</v>
+      </c>
+      <c r="D93" s="15">
+        <v>1</v>
+      </c>
+      <c r="E93" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G93" s="14">
+        <v>22</v>
+      </c>
+      <c r="H93" s="14">
+        <v>2</v>
+      </c>
+      <c r="I93" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="J93" s="14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B94" s="15">
+        <v>1</v>
+      </c>
+      <c r="C94" s="15">
+        <v>1</v>
+      </c>
+      <c r="D94" s="15">
+        <v>1</v>
+      </c>
+      <c r="E94" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G94" s="14">
+        <v>22</v>
+      </c>
+      <c r="H94" s="14">
+        <v>2</v>
+      </c>
+      <c r="I94" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="J94" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B95" s="15">
+        <v>1</v>
+      </c>
+      <c r="C95" s="15">
+        <v>1</v>
+      </c>
+      <c r="D95" s="15">
+        <v>1</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G95" s="4">
+        <v>21</v>
+      </c>
+      <c r="H95" s="4">
+        <v>0</v>
+      </c>
+      <c r="I95" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B96" s="15">
+        <v>1</v>
+      </c>
+      <c r="C96" s="15">
+        <v>1</v>
+      </c>
+      <c r="D96" s="15">
+        <v>1</v>
+      </c>
+      <c r="E96" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G96" s="4">
+        <v>23</v>
+      </c>
+      <c r="H96" s="4">
+        <v>0</v>
+      </c>
+      <c r="I96" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="J96" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="75">
+      <c r="A97" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B97" s="15">
+        <v>1</v>
+      </c>
+      <c r="C97" s="15">
+        <v>1</v>
+      </c>
+      <c r="D97" s="15">
+        <v>1</v>
+      </c>
+      <c r="E97" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G97" s="14">
+        <v>21</v>
+      </c>
+      <c r="H97" s="14">
+        <v>0</v>
+      </c>
+      <c r="I97" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="J97" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="47.25">
+      <c r="A98" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B98" s="15">
+        <v>1</v>
+      </c>
+      <c r="C98" s="15">
+        <v>1</v>
+      </c>
+      <c r="D98" s="15">
+        <v>1</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G98" s="4">
+        <v>29</v>
+      </c>
+      <c r="H98" s="4">
+        <v>1</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="J98" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="78.75">
+      <c r="A99" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B99" s="15">
+        <v>1</v>
+      </c>
+      <c r="C99" s="15">
+        <v>1</v>
+      </c>
+      <c r="D99" s="15">
+        <v>1</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G99" s="4">
+        <v>24</v>
+      </c>
+      <c r="H99" s="4">
+        <v>1</v>
+      </c>
+      <c r="I99" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="J99" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="31.5">
+      <c r="A100" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B100" s="15">
+        <v>1</v>
+      </c>
+      <c r="C100" s="15">
+        <v>1</v>
+      </c>
+      <c r="D100" s="15">
+        <v>1</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G100" s="4">
+        <v>30</v>
+      </c>
+      <c r="H100" s="4">
+        <v>0</v>
+      </c>
+      <c r="I100" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="J100" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="63">
+      <c r="A101" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B101" s="15">
+        <v>1</v>
+      </c>
+      <c r="C101" s="15">
+        <v>1</v>
+      </c>
+      <c r="D101" s="15">
+        <v>1</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G101" s="4">
+        <v>29</v>
+      </c>
+      <c r="H101" s="4">
+        <v>1</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="J101" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="63">
+      <c r="A102" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B102" s="15">
+        <v>1</v>
+      </c>
+      <c r="C102" s="15">
+        <v>1</v>
+      </c>
+      <c r="D102" s="15">
+        <v>1</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G102" s="4">
+        <v>23</v>
+      </c>
+      <c r="H102" s="4">
+        <v>1</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="J102" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B103" s="3">
+        <v>0</v>
+      </c>
+      <c r="C103" s="15">
+        <v>1</v>
+      </c>
+      <c r="D103" s="3">
+        <v>0</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" s="4">
+        <v>23</v>
+      </c>
+      <c r="H103" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="126">
+      <c r="A104" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B104" s="15">
+        <v>1</v>
+      </c>
+      <c r="C104" s="15">
+        <v>1</v>
+      </c>
+      <c r="D104" s="15">
+        <v>1</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G104" s="4">
+        <v>34</v>
+      </c>
+      <c r="H104" s="4">
+        <v>1</v>
+      </c>
+      <c r="I104" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="J104" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="63">
+      <c r="A105" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B105" s="3">
+        <v>0</v>
+      </c>
+      <c r="C105" s="15">
+        <v>1</v>
+      </c>
+      <c r="D105" s="3">
+        <v>0</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G105" s="4">
+        <v>22</v>
+      </c>
+      <c r="H105" s="4">
+        <v>0</v>
+      </c>
+      <c r="I105" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="J105" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="47.25">
+      <c r="A106" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B106" s="15">
+        <v>1</v>
+      </c>
+      <c r="C106" s="15">
+        <v>1</v>
+      </c>
+      <c r="D106" s="15">
+        <v>1</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G106" s="4">
+        <v>22</v>
+      </c>
+      <c r="H106" s="4">
+        <v>1</v>
+      </c>
+      <c r="I106" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="J106" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B107" s="15">
+        <v>1</v>
+      </c>
+      <c r="C107" s="15">
+        <v>1</v>
+      </c>
+      <c r="D107" s="15">
+        <v>1</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G107" s="4">
+        <v>22</v>
+      </c>
+      <c r="H107" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="94.5">
+      <c r="A108" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B108" s="15">
+        <v>1</v>
+      </c>
+      <c r="C108" s="15">
+        <v>1</v>
+      </c>
+      <c r="D108" s="15">
+        <v>1</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G108" s="4">
+        <v>18</v>
+      </c>
+      <c r="H108" s="4">
+        <v>1</v>
+      </c>
+      <c r="I108" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J108" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B109" s="15">
+        <v>1</v>
+      </c>
+      <c r="C109" s="15">
+        <v>1</v>
+      </c>
+      <c r="D109" s="15">
+        <v>1</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G109" s="4">
+        <v>23</v>
+      </c>
+      <c r="H109" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B110" s="15">
+        <v>1</v>
+      </c>
+      <c r="C110" s="15">
+        <v>1</v>
+      </c>
+      <c r="D110" s="15">
+        <v>1</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G110" s="4">
+        <v>22</v>
+      </c>
+      <c r="H110" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B111" s="15">
+        <v>1</v>
+      </c>
+      <c r="C111" s="15">
+        <v>1</v>
+      </c>
+      <c r="D111" s="15">
+        <v>1</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G111" s="4">
+        <v>19</v>
+      </c>
+      <c r="H111" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="47.25">
+      <c r="A112" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B112" s="15">
+        <v>1</v>
+      </c>
+      <c r="C112" s="15">
+        <v>1</v>
+      </c>
+      <c r="D112" s="15">
+        <v>1</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G112" s="4">
+        <v>22</v>
+      </c>
+      <c r="H112" s="4">
+        <v>1</v>
+      </c>
+      <c r="I112" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="J112" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="47.25">
+      <c r="A113" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B113" s="15">
+        <v>1</v>
+      </c>
+      <c r="C113" s="15">
+        <v>1</v>
+      </c>
+      <c r="D113" s="15">
+        <v>1</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G113" s="4">
+        <v>22</v>
+      </c>
+      <c r="H113" s="4">
+        <v>0</v>
+      </c>
+      <c r="I113" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="J113" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="78.75">
+      <c r="A114" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B114" s="15">
+        <v>1</v>
+      </c>
+      <c r="C114" s="15">
+        <v>1</v>
+      </c>
+      <c r="D114" s="15">
+        <v>1</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G114" s="4">
+        <v>20</v>
+      </c>
+      <c r="H114" s="4">
+        <v>1</v>
+      </c>
+      <c r="I114" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="J114" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="157.5">
+      <c r="A115" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B115" s="15">
+        <v>1</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G115" s="4">
+        <v>22</v>
+      </c>
+      <c r="H115" s="4">
+        <v>1</v>
+      </c>
+      <c r="I115" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="J115" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:J127">
+    <sortCondition ref="C2:C127"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update medication info and effect size analysis of questionnaires
</commit_message>
<xml_diff>
--- a/data/Demographics.xlsx
+++ b/data/Demographics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11475" yWindow="1200" windowWidth="28245" windowHeight="17235" activeTab="5"/>
+    <workbookView xWindow="11475" yWindow="1200" windowWidth="28245" windowHeight="17235" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="MDD_EEG Analysis" sheetId="3" r:id="rId4"/>
     <sheet name="MDD_fMRI Analysis" sheetId="6" r:id="rId5"/>
     <sheet name="fMRT_RT_Analysis" sheetId="7" r:id="rId6"/>
+    <sheet name="Tabelle1" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="256">
   <si>
     <t>Healthy Control (HC) or Patient</t>
   </si>
@@ -915,6 +916,58 @@
   </si>
   <si>
     <t>F33.1 rez. Depr. Mittel</t>
+  </si>
+  <si>
+    <t>SSRI</t>
+  </si>
+  <si>
+    <t>SNDRI</t>
+  </si>
+  <si>
+    <t>morning:  Elontril 300mg
+evening: Quetiapin 100mg
+night: Quetiapin 100mg</t>
+  </si>
+  <si>
+    <t>SNDRI, SSRI</t>
+  </si>
+  <si>
+    <t>SSRI, AAP</t>
+  </si>
+  <si>
+    <t>SNDRI,  AAP</t>
+  </si>
+  <si>
+    <t>SNRI</t>
+  </si>
+  <si>
+    <t>AAD</t>
+  </si>
+  <si>
+    <t>SSRI,NaSSA</t>
+  </si>
+  <si>
+    <t>NaSSA</t>
+  </si>
+  <si>
+    <t>SNRI,AAP,NaSSA</t>
+  </si>
+  <si>
+    <t>NDRI</t>
+  </si>
+  <si>
+    <t>Group of Antidepressants 
+SSRI = selective serotonin reuptake inhibitors
+SNRI = serotonin and norepinephrine reuptake inhibitors 
+MAO = monoamine oxidase inhibitors
+SNDRI = serotonin–norepinephrine–dopamine reuptake inhibitor
+NaSSA = noradrenergic and specific serotonergic antidepressant
+AAP = atypical antipsychotic
+AAD = atypical antidepressant
+NDRI = Norepinephrine-Dopamine Reuptake Inhibitor</t>
+  </si>
+  <si>
+    <t>SSRI, NaSSA</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1217,6 +1270,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12414,10 +12470,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" activeCellId="4" sqref="A1:A1048576 E1:E1048576 F1:F1048576 G1:G1048576 H1:H1048576"/>
+    <sheetView topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15.75"/>
@@ -12430,12 +12486,13 @@
     <col min="6" max="6" width="9" style="4" customWidth="1"/>
     <col min="7" max="7" width="11.875" style="4" customWidth="1"/>
     <col min="8" max="8" width="16" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="53.125" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="9.125" style="4"/>
+    <col min="9" max="9" width="21.125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="24.375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="53.125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="9.125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="19" customFormat="1" ht="30">
+    <row r="1" spans="1:11" s="19" customFormat="1" ht="75.75" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
@@ -12461,13 +12518,16 @@
         <v>236</v>
       </c>
       <c r="I1" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -12493,9 +12553,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="J2" s="2"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -12521,9 +12582,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="2"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="60">
+      <c r="J3" s="2"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="60">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -12549,13 +12611,16 @@
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="45">
+    <row r="5" spans="1:11" ht="45">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -12581,13 +12646,16 @@
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45">
+    <row r="6" spans="1:11" ht="45">
       <c r="A6" s="5" t="s">
         <v>17</v>
       </c>
@@ -12613,13 +12681,16 @@
         <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -12645,9 +12716,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="J7" s="2"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -12673,9 +12745,10 @@
         <v>0</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="60">
+      <c r="J8" s="2"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="45">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
@@ -12701,13 +12774,16 @@
         <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="J9" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -12733,9 +12809,10 @@
         <v>0</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10" s="2"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -12761,9 +12838,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="2"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="J11" s="2"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="8" t="s">
         <v>26</v>
       </c>
@@ -12789,9 +12867,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="J12" s="2"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="8" t="s">
         <v>27</v>
       </c>
@@ -12817,9 +12896,10 @@
         <v>0</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="J13" s="2"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="8" t="s">
         <v>28</v>
       </c>
@@ -12845,9 +12925,10 @@
         <v>0</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="J14" s="2"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
@@ -12873,9 +12954,10 @@
         <v>0</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="J15" s="2"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="8" t="s">
         <v>32</v>
       </c>
@@ -12901,9 +12983,10 @@
         <v>0</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="J16" s="2"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="8" t="s">
         <v>33</v>
       </c>
@@ -12929,9 +13012,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="J17" s="2"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="8" t="s">
         <v>34</v>
       </c>
@@ -12957,9 +13041,10 @@
         <v>0</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" ht="45">
+      <c r="J18" s="2"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" ht="45">
       <c r="A19" s="9" t="s">
         <v>35</v>
       </c>
@@ -12985,13 +13070,16 @@
         <v>1</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:11">
       <c r="A20" s="8" t="s">
         <v>37</v>
       </c>
@@ -13017,9 +13105,10 @@
         <v>0</v>
       </c>
       <c r="I20" s="2"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="J20" s="2"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="8" t="s">
         <v>38</v>
       </c>
@@ -13045,9 +13134,10 @@
         <v>0</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="J21" s="2"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="8" t="s">
         <v>39</v>
       </c>
@@ -13073,9 +13163,10 @@
         <v>0</v>
       </c>
       <c r="I22" s="2"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="J22" s="2"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="8" t="s">
         <v>40</v>
       </c>
@@ -13101,9 +13192,10 @@
         <v>0</v>
       </c>
       <c r="I23" s="2"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="J23" s="2"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="8" t="s">
         <v>41</v>
       </c>
@@ -13129,9 +13221,10 @@
         <v>0</v>
       </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="J24" s="2"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="8" t="s">
         <v>42</v>
       </c>
@@ -13157,9 +13250,10 @@
         <v>0</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="J25" s="2"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="8" t="s">
         <v>43</v>
       </c>
@@ -13185,9 +13279,10 @@
         <v>0</v>
       </c>
       <c r="I26" s="2"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="J26" s="2"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="8" t="s">
         <v>44</v>
       </c>
@@ -13213,9 +13308,10 @@
         <v>0</v>
       </c>
       <c r="I27" s="2"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" ht="60">
+      <c r="J27" s="2"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" ht="60">
       <c r="A28" s="9" t="s">
         <v>45</v>
       </c>
@@ -13240,14 +13336,15 @@
       <c r="H28" s="2">
         <v>0</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" s="2"/>
+      <c r="J28" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="60">
+    <row r="29" spans="1:11" ht="60">
       <c r="A29" s="9" t="s">
         <v>47</v>
       </c>
@@ -13273,13 +13370,16 @@
         <v>1</v>
       </c>
       <c r="I29" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="45">
+    <row r="30" spans="1:11" ht="45">
       <c r="A30" s="9" t="s">
         <v>49</v>
       </c>
@@ -13304,14 +13404,15 @@
       <c r="H30" s="2">
         <v>0</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="2"/>
+      <c r="J30" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="60">
+    <row r="31" spans="1:11" ht="60">
       <c r="A31" s="9" t="s">
         <v>51</v>
       </c>
@@ -13336,14 +13437,15 @@
       <c r="H31" s="2">
         <v>0</v>
       </c>
-      <c r="I31" s="2" t="s">
+      <c r="I31" s="2"/>
+      <c r="J31" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:11">
       <c r="A32" s="9" t="s">
         <v>53</v>
       </c>
@@ -13369,13 +13471,16 @@
         <v>1</v>
       </c>
       <c r="I32" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="60">
+    <row r="33" spans="1:11" ht="60">
       <c r="A33" s="9" t="s">
         <v>55</v>
       </c>
@@ -13400,14 +13505,15 @@
       <c r="H33" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="I33" s="2"/>
+      <c r="J33" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:11">
       <c r="A34" s="11" t="s">
         <v>57</v>
       </c>
@@ -13433,9 +13539,10 @@
         <v>0</v>
       </c>
       <c r="I34" s="2"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="J34" s="2"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="8" t="s">
         <v>60</v>
       </c>
@@ -13461,9 +13568,10 @@
         <v>0</v>
       </c>
       <c r="I35" s="2"/>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="J35" s="2"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="9" t="s">
         <v>61</v>
       </c>
@@ -13489,13 +13597,16 @@
         <v>1</v>
       </c>
       <c r="I36" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:11">
       <c r="A37" s="8" t="s">
         <v>63</v>
       </c>
@@ -13521,9 +13632,10 @@
         <v>0</v>
       </c>
       <c r="I37" s="2"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="J37" s="2"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="8" t="s">
         <v>64</v>
       </c>
@@ -13549,9 +13661,10 @@
         <v>0</v>
       </c>
       <c r="I38" s="2"/>
-      <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="J38" s="2"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="8" t="s">
         <v>65</v>
       </c>
@@ -13577,9 +13690,10 @@
         <v>0</v>
       </c>
       <c r="I39" s="2"/>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" ht="60">
+      <c r="J39" s="2"/>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:11" ht="60">
       <c r="A40" s="9" t="s">
         <v>66</v>
       </c>
@@ -13605,13 +13719,16 @@
         <v>1</v>
       </c>
       <c r="I40" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="K40" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="60">
+    <row r="41" spans="1:11" ht="60">
       <c r="A41" s="9" t="s">
         <v>68</v>
       </c>
@@ -13637,13 +13754,16 @@
         <v>1</v>
       </c>
       <c r="I41" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="J41" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="K41" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:11">
       <c r="A42" s="37" t="s">
         <v>70</v>
       </c>
@@ -13669,9 +13789,10 @@
         <v>0</v>
       </c>
       <c r="I42" s="2"/>
-      <c r="J42" s="1"/>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="J42" s="2"/>
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="8" t="s">
         <v>71</v>
       </c>
@@ -13697,9 +13818,10 @@
         <v>0</v>
       </c>
       <c r="I43" s="2"/>
-      <c r="J43" s="1"/>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="J43" s="2"/>
+      <c r="K43" s="1"/>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="8" t="s">
         <v>72</v>
       </c>
@@ -13725,9 +13847,10 @@
         <v>0</v>
       </c>
       <c r="I44" s="2"/>
-      <c r="J44" s="1"/>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="J44" s="2"/>
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="8" t="s">
         <v>73</v>
       </c>
@@ -13753,9 +13876,10 @@
         <v>0</v>
       </c>
       <c r="I45" s="2"/>
-      <c r="J45" s="1"/>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="J45" s="2"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="8" t="s">
         <v>74</v>
       </c>
@@ -13781,9 +13905,10 @@
         <v>0</v>
       </c>
       <c r="I46" s="2"/>
-      <c r="J46" s="1"/>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="J46" s="2"/>
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="8" t="s">
         <v>75</v>
       </c>
@@ -13809,9 +13934,10 @@
         <v>0</v>
       </c>
       <c r="I47" s="2"/>
-      <c r="J47" s="1"/>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="J47" s="2"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="8" t="s">
         <v>76</v>
       </c>
@@ -13837,9 +13963,10 @@
         <v>0</v>
       </c>
       <c r="I48" s="2"/>
-      <c r="J48" s="1"/>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="J48" s="2"/>
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="8" t="s">
         <v>77</v>
       </c>
@@ -13865,9 +13992,10 @@
         <v>0</v>
       </c>
       <c r="I49" s="2"/>
-      <c r="J49" s="1"/>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="J49" s="2"/>
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="8" t="s">
         <v>79</v>
       </c>
@@ -13893,9 +14021,10 @@
         <v>0</v>
       </c>
       <c r="I50" s="2"/>
-      <c r="J50" s="1"/>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="J50" s="2"/>
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="8" t="s">
         <v>84</v>
       </c>
@@ -13921,9 +14050,10 @@
         <v>0</v>
       </c>
       <c r="I51" s="2"/>
-      <c r="J51" s="1"/>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="J51" s="2"/>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="9" t="s">
         <v>86</v>
       </c>
@@ -13948,14 +14078,15 @@
       <c r="H52" s="2">
         <v>0</v>
       </c>
-      <c r="I52" s="2" t="s">
+      <c r="I52" s="2"/>
+      <c r="J52" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="K52" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="45">
+    <row r="53" spans="1:11" ht="45">
       <c r="A53" s="9" t="s">
         <v>87</v>
       </c>
@@ -13981,13 +14112,16 @@
         <v>1</v>
       </c>
       <c r="I53" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J53" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="J53" s="1" t="s">
+      <c r="K53" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="60">
+    <row r="54" spans="1:11" ht="60">
       <c r="A54" s="12" t="s">
         <v>89</v>
       </c>
@@ -14012,14 +14146,15 @@
       <c r="H54" s="2">
         <v>0</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="I54" s="2"/>
+      <c r="J54" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J54" s="1" t="s">
+      <c r="K54" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="30">
+    <row r="55" spans="1:11" ht="30">
       <c r="A55" s="12" t="s">
         <v>91</v>
       </c>
@@ -14045,13 +14180,16 @@
         <v>1</v>
       </c>
       <c r="I55" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="J55" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:11">
       <c r="A56" s="8" t="s">
         <v>93</v>
       </c>
@@ -14077,9 +14215,10 @@
         <v>0</v>
       </c>
       <c r="I56" s="2"/>
-      <c r="J56" s="1"/>
-    </row>
-    <row r="57" spans="1:10">
+      <c r="J56" s="2"/>
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="8" t="s">
         <v>94</v>
       </c>
@@ -14105,9 +14244,10 @@
         <v>0</v>
       </c>
       <c r="I57" s="2"/>
-      <c r="J57" s="1"/>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="J57" s="2"/>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="8" t="s">
         <v>95</v>
       </c>
@@ -14133,9 +14273,10 @@
         <v>0</v>
       </c>
       <c r="I58" s="2"/>
-      <c r="J58" s="1"/>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="J58" s="2"/>
+      <c r="K58" s="1"/>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="8" t="s">
         <v>96</v>
       </c>
@@ -14161,9 +14302,10 @@
         <v>0</v>
       </c>
       <c r="I59" s="2"/>
-      <c r="J59" s="1"/>
-    </row>
-    <row r="60" spans="1:10" ht="30">
+      <c r="J59" s="2"/>
+      <c r="K59" s="1"/>
+    </row>
+    <row r="60" spans="1:11" ht="30">
       <c r="A60" s="9" t="s">
         <v>97</v>
       </c>
@@ -14189,13 +14331,16 @@
         <v>1</v>
       </c>
       <c r="I60" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="J60" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="J60" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:11">
       <c r="A61" s="8" t="s">
         <v>99</v>
       </c>
@@ -14221,9 +14366,10 @@
         <v>0</v>
       </c>
       <c r="I61" s="2"/>
-      <c r="J61" s="1"/>
-    </row>
-    <row r="62" spans="1:10">
+      <c r="J61" s="2"/>
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="8" t="s">
         <v>100</v>
       </c>
@@ -14249,9 +14395,10 @@
         <v>0</v>
       </c>
       <c r="I62" s="2"/>
-      <c r="J62" s="1"/>
-    </row>
-    <row r="63" spans="1:10" ht="45">
+      <c r="J62" s="2"/>
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="1:11" ht="45">
       <c r="A63" s="9" t="s">
         <v>101</v>
       </c>
@@ -14276,14 +14423,15 @@
       <c r="H63" s="2">
         <v>1</v>
       </c>
-      <c r="I63" s="2" t="s">
+      <c r="I63" s="2"/>
+      <c r="J63" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="J63" s="1" t="s">
+      <c r="K63" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="30">
+    <row r="64" spans="1:11" ht="30">
       <c r="A64" s="9" t="s">
         <v>103</v>
       </c>
@@ -14308,14 +14456,15 @@
       <c r="H64" s="2">
         <v>0</v>
       </c>
-      <c r="I64" s="2" t="s">
+      <c r="I64" s="2"/>
+      <c r="J64" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J64" s="1" t="s">
+      <c r="K64" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:11">
       <c r="A65" s="9" t="s">
         <v>105</v>
       </c>
@@ -14340,14 +14489,15 @@
       <c r="H65" s="2">
         <v>0</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="I65" s="2"/>
+      <c r="J65" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J65" s="1" t="s">
+      <c r="K65" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:11">
       <c r="A66" s="8" t="s">
         <v>107</v>
       </c>
@@ -14373,9 +14523,10 @@
         <v>0</v>
       </c>
       <c r="I66" s="2"/>
-      <c r="J66" s="1"/>
-    </row>
-    <row r="67" spans="1:10">
+      <c r="J66" s="2"/>
+      <c r="K66" s="1"/>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" s="8" t="s">
         <v>108</v>
       </c>
@@ -14401,9 +14552,10 @@
         <v>0</v>
       </c>
       <c r="I67" s="2"/>
-      <c r="J67" s="1"/>
-    </row>
-    <row r="68" spans="1:10" ht="105">
+      <c r="J67" s="2"/>
+      <c r="K67" s="1"/>
+    </row>
+    <row r="68" spans="1:11" ht="105">
       <c r="A68" s="9" t="s">
         <v>109</v>
       </c>
@@ -14429,13 +14581,16 @@
         <v>1</v>
       </c>
       <c r="I68" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J68" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="J68" s="1" t="s">
+      <c r="K68" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="30">
+    <row r="69" spans="1:11" ht="30">
       <c r="A69" s="9" t="s">
         <v>111</v>
       </c>
@@ -14461,13 +14616,16 @@
         <v>1</v>
       </c>
       <c r="I69" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J69" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="J69" s="1" t="s">
+      <c r="K69" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:11">
       <c r="A70" s="8" t="s">
         <v>113</v>
       </c>
@@ -14493,9 +14651,10 @@
         <v>0</v>
       </c>
       <c r="I70" s="2"/>
-      <c r="J70" s="1"/>
-    </row>
-    <row r="71" spans="1:10" ht="45">
+      <c r="J70" s="2"/>
+      <c r="K70" s="1"/>
+    </row>
+    <row r="71" spans="1:11" ht="45">
       <c r="A71" s="9" t="s">
         <v>114</v>
       </c>
@@ -14521,13 +14680,16 @@
         <v>1</v>
       </c>
       <c r="I71" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J71" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="J71" s="1" t="s">
+      <c r="K71" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:11">
       <c r="A72" s="8" t="s">
         <v>116</v>
       </c>
@@ -14553,9 +14715,10 @@
         <v>0</v>
       </c>
       <c r="I72" s="2"/>
-      <c r="J72" s="1"/>
-    </row>
-    <row r="73" spans="1:10">
+      <c r="J72" s="2"/>
+      <c r="K72" s="1"/>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="8" t="s">
         <v>117</v>
       </c>
@@ -14581,9 +14744,10 @@
         <v>0</v>
       </c>
       <c r="I73" s="2"/>
-      <c r="J73" s="1"/>
-    </row>
-    <row r="74" spans="1:10" ht="60">
+      <c r="J73" s="2"/>
+      <c r="K73" s="1"/>
+    </row>
+    <row r="74" spans="1:11" ht="60">
       <c r="A74" s="9" t="s">
         <v>118</v>
       </c>
@@ -14609,13 +14773,16 @@
         <v>1</v>
       </c>
       <c r="I74" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J74" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="J74" s="1" t="s">
+      <c r="K74" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:11">
       <c r="A75" s="8" t="s">
         <v>120</v>
       </c>
@@ -14641,9 +14808,10 @@
         <v>0</v>
       </c>
       <c r="I75" s="2"/>
-      <c r="J75" s="1"/>
-    </row>
-    <row r="76" spans="1:10">
+      <c r="J75" s="2"/>
+      <c r="K75" s="1"/>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="8" t="s">
         <v>121</v>
       </c>
@@ -14669,9 +14837,10 @@
         <v>0</v>
       </c>
       <c r="I76" s="2"/>
-      <c r="J76" s="1"/>
-    </row>
-    <row r="77" spans="1:10">
+      <c r="J76" s="2"/>
+      <c r="K76" s="1"/>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="8" t="s">
         <v>122</v>
       </c>
@@ -14697,9 +14866,10 @@
         <v>0</v>
       </c>
       <c r="I77" s="2"/>
-      <c r="J77" s="1"/>
-    </row>
-    <row r="78" spans="1:10">
+      <c r="J77" s="2"/>
+      <c r="K77" s="1"/>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="8" t="s">
         <v>123</v>
       </c>
@@ -14725,9 +14895,10 @@
         <v>0</v>
       </c>
       <c r="I78" s="2"/>
-      <c r="J78" s="1"/>
-    </row>
-    <row r="79" spans="1:10" ht="47.25">
+      <c r="J78" s="2"/>
+      <c r="K78" s="1"/>
+    </row>
+    <row r="79" spans="1:11" ht="47.25">
       <c r="A79" s="13" t="s">
         <v>124</v>
       </c>
@@ -14753,13 +14924,16 @@
         <v>1</v>
       </c>
       <c r="I79" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J79" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="J79" s="4" t="s">
+      <c r="K79" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:11">
       <c r="A80" s="8" t="s">
         <v>126</v>
       </c>
@@ -14785,8 +14959,9 @@
         <v>0</v>
       </c>
       <c r="I80" s="2"/>
-    </row>
-    <row r="81" spans="1:10" ht="31.5">
+      <c r="J80" s="2"/>
+    </row>
+    <row r="81" spans="1:11" ht="31.5">
       <c r="A81" s="13" t="s">
         <v>129</v>
       </c>
@@ -14812,13 +14987,16 @@
         <v>1</v>
       </c>
       <c r="I81" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J81" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="J81" s="4" t="s">
+      <c r="K81" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:11">
       <c r="A82" s="8" t="s">
         <v>131</v>
       </c>
@@ -14843,8 +15021,9 @@
       <c r="H82" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" ht="45">
+      <c r="I82" s="2"/>
+    </row>
+    <row r="83" spans="1:11" ht="45">
       <c r="A83" s="13" t="s">
         <v>132</v>
       </c>
@@ -14870,13 +15049,16 @@
         <v>1</v>
       </c>
       <c r="I83" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="J83" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="2" t="s">
+      <c r="K83" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="16.5" customHeight="1">
+    <row r="84" spans="1:11" ht="16.5" customHeight="1">
       <c r="A84" s="13" t="s">
         <v>134</v>
       </c>
@@ -14901,14 +15083,15 @@
       <c r="H84" s="2">
         <v>0</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="I84" s="2"/>
+      <c r="J84" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J84" s="2" t="s">
+      <c r="K84" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="30">
+    <row r="85" spans="1:11" ht="30">
       <c r="A85" s="13" t="s">
         <v>136</v>
       </c>
@@ -14933,14 +15116,15 @@
       <c r="H85" s="2">
         <v>0</v>
       </c>
-      <c r="I85" s="2" t="s">
+      <c r="I85" s="2"/>
+      <c r="J85" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J85" s="10" t="s">
+      <c r="K85" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="47.25">
+    <row r="86" spans="1:11" ht="47.25">
       <c r="A86" s="13" t="s">
         <v>138</v>
       </c>
@@ -14965,14 +15149,15 @@
       <c r="H86" s="2">
         <v>0</v>
       </c>
-      <c r="I86" s="2" t="s">
+      <c r="I86" s="2"/>
+      <c r="J86" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="J86" s="4" t="s">
+      <c r="K86" s="4" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="110.25">
+    <row r="87" spans="1:11" ht="110.25">
       <c r="A87" s="13" t="s">
         <v>140</v>
       </c>
@@ -14998,13 +15183,16 @@
         <v>1</v>
       </c>
       <c r="I87" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="J87" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="J87" s="4" t="s">
+      <c r="K87" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:11">
       <c r="A88" s="8" t="s">
         <v>142</v>
       </c>
@@ -15030,8 +15218,9 @@
         <v>0</v>
       </c>
       <c r="I88" s="2"/>
-    </row>
-    <row r="89" spans="1:10" ht="94.5">
+      <c r="J88" s="2"/>
+    </row>
+    <row r="89" spans="1:11" ht="94.5">
       <c r="A89" s="13" t="s">
         <v>143</v>
       </c>
@@ -15056,14 +15245,15 @@
       <c r="H89" s="2">
         <v>0</v>
       </c>
-      <c r="I89" s="2" t="s">
+      <c r="I89" s="2"/>
+      <c r="J89" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="J89" s="4" t="s">
+      <c r="K89" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="78.75">
+    <row r="90" spans="1:11" ht="78.75">
       <c r="A90" s="13" t="s">
         <v>146</v>
       </c>
@@ -15089,13 +15279,16 @@
         <v>1</v>
       </c>
       <c r="I90" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="J90" s="4" t="s">
+      <c r="K90" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="78.75">
+    <row r="91" spans="1:11" ht="78.75">
       <c r="A91" s="13" t="s">
         <v>148</v>
       </c>
@@ -15120,14 +15313,17 @@
       <c r="H91" s="4">
         <v>1</v>
       </c>
-      <c r="I91" s="4" t="s">
+      <c r="I91" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J91" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="J91" s="4" t="s">
+      <c r="K91" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="63">
+    <row r="92" spans="1:11" ht="63">
       <c r="A92" s="13" t="s">
         <v>150</v>
       </c>
@@ -15150,16 +15346,19 @@
         <v>26</v>
       </c>
       <c r="H92" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I92" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="J92" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="J92" s="4" t="s">
+      <c r="K92" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="60">
+    <row r="93" spans="1:11" ht="60">
       <c r="A93" s="13" t="s">
         <v>152</v>
       </c>
@@ -15182,16 +15381,19 @@
         <v>22</v>
       </c>
       <c r="H93" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I93" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="J93" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="J93" s="14" t="s">
+      <c r="K93" s="14" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:11">
       <c r="A94" s="13" t="s">
         <v>154</v>
       </c>
@@ -15214,16 +15416,19 @@
         <v>22</v>
       </c>
       <c r="H94" s="14">
-        <v>2</v>
-      </c>
-      <c r="I94" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I94" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J94" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="J94" s="14" t="s">
+      <c r="K94" s="14" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:11">
       <c r="A95" s="13" t="s">
         <v>156</v>
       </c>
@@ -15248,14 +15453,14 @@
       <c r="H95" s="4">
         <v>0</v>
       </c>
-      <c r="I95" s="4" t="s">
+      <c r="J95" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="J95" s="4" t="s">
+      <c r="K95" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:11">
       <c r="A96" s="13" t="s">
         <v>158</v>
       </c>
@@ -15280,14 +15485,14 @@
       <c r="H96" s="4">
         <v>0</v>
       </c>
-      <c r="I96" s="4" t="s">
+      <c r="J96" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="J96" s="2" t="s">
+      <c r="K96" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="75">
+    <row r="97" spans="1:11" ht="75">
       <c r="A97" s="13" t="s">
         <v>159</v>
       </c>
@@ -15312,14 +15517,15 @@
       <c r="H97" s="14">
         <v>0</v>
       </c>
-      <c r="I97" s="14" t="s">
+      <c r="I97" s="14"/>
+      <c r="J97" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="J97" s="14" t="s">
+      <c r="K97" s="14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="47.25">
+    <row r="98" spans="1:11" ht="47.25">
       <c r="A98" s="13" t="s">
         <v>161</v>
       </c>
@@ -15345,13 +15551,16 @@
         <v>1</v>
       </c>
       <c r="I98" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="J98" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="J98" s="4" t="s">
+      <c r="K98" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="78.75">
+    <row r="99" spans="1:11" ht="78.75">
       <c r="A99" s="13" t="s">
         <v>163</v>
       </c>
@@ -15377,13 +15586,16 @@
         <v>1</v>
       </c>
       <c r="I99" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="J99" s="4" t="s">
+      <c r="K99" s="4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="31.5">
+    <row r="100" spans="1:11" ht="31.5">
       <c r="A100" s="13" t="s">
         <v>165</v>
       </c>
@@ -15408,14 +15620,14 @@
       <c r="H100" s="4">
         <v>0</v>
       </c>
-      <c r="I100" s="4" t="s">
+      <c r="J100" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="J100" s="4" t="s">
+      <c r="K100" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="63">
+    <row r="101" spans="1:11" ht="63">
       <c r="A101" s="13" t="s">
         <v>167</v>
       </c>
@@ -15441,13 +15653,16 @@
         <v>1</v>
       </c>
       <c r="I101" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="J101" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="J101" s="4" t="s">
+      <c r="K101" s="4" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="63">
+    <row r="102" spans="1:11" ht="63">
       <c r="A102" s="13" t="s">
         <v>169</v>
       </c>
@@ -15472,14 +15687,17 @@
       <c r="H102" s="4">
         <v>1</v>
       </c>
-      <c r="I102" s="4" t="s">
+      <c r="I102" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="J102" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="J102" s="4" t="s">
+      <c r="K102" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:11">
       <c r="A103" s="8" t="s">
         <v>171</v>
       </c>
@@ -15505,7 +15723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="126">
+    <row r="104" spans="1:11" ht="126">
       <c r="A104" s="13" t="s">
         <v>172</v>
       </c>
@@ -15531,13 +15749,16 @@
         <v>1</v>
       </c>
       <c r="I104" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="J104" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="J104" s="4" t="s">
+      <c r="K104" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="63">
+    <row r="105" spans="1:11" ht="63">
       <c r="A105" s="13" t="s">
         <v>174</v>
       </c>
@@ -15562,14 +15783,14 @@
       <c r="H105" s="4">
         <v>0</v>
       </c>
-      <c r="I105" s="4" t="s">
+      <c r="J105" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="J105" s="4" t="s">
+      <c r="K105" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="47.25">
+    <row r="106" spans="1:11" ht="47.25">
       <c r="A106" s="13" t="s">
         <v>176</v>
       </c>
@@ -15595,13 +15816,16 @@
         <v>1</v>
       </c>
       <c r="I106" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="J106" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="J106" s="4" t="s">
+      <c r="K106" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:11">
       <c r="A107" s="8" t="s">
         <v>178</v>
       </c>
@@ -15627,7 +15851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="94.5">
+    <row r="108" spans="1:11" ht="94.5">
       <c r="A108" s="13" t="s">
         <v>180</v>
       </c>
@@ -15653,13 +15877,16 @@
         <v>1</v>
       </c>
       <c r="I108" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="J108" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="J108" s="4" t="s">
+      <c r="K108" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:11">
       <c r="A109" s="8" t="s">
         <v>182</v>
       </c>
@@ -15685,7 +15912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:11">
       <c r="A110" s="8" t="s">
         <v>183</v>
       </c>
@@ -15711,7 +15938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:11">
       <c r="A111" s="8" t="s">
         <v>184</v>
       </c>
@@ -15737,7 +15964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="47.25">
+    <row r="112" spans="1:11" ht="47.25">
       <c r="A112" s="13" t="s">
         <v>185</v>
       </c>
@@ -15763,13 +15990,16 @@
         <v>1</v>
       </c>
       <c r="I112" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="J112" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="J112" s="4" t="s">
+      <c r="K112" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="47.25">
+    <row r="113" spans="1:11" ht="47.25">
       <c r="A113" s="13" t="s">
         <v>187</v>
       </c>
@@ -15794,14 +16024,14 @@
       <c r="H113" s="4">
         <v>0</v>
       </c>
-      <c r="I113" s="4" t="s">
+      <c r="J113" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="J113" s="4" t="s">
+      <c r="K113" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="78.75">
+    <row r="114" spans="1:11" ht="78.75">
       <c r="A114" s="13" t="s">
         <v>189</v>
       </c>
@@ -15827,13 +16057,16 @@
         <v>1</v>
       </c>
       <c r="I114" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="J114" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="J114" s="4" t="s">
+      <c r="K114" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="157.5">
+    <row r="115" spans="1:11" ht="157.5">
       <c r="A115" s="13" t="s">
         <v>191</v>
       </c>
@@ -15858,10 +16091,13 @@
       <c r="H115" s="4">
         <v>1</v>
       </c>
-      <c r="I115" s="4" t="s">
+      <c r="I115" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="J115" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="J115" s="4" t="s">
+      <c r="K115" s="4" t="s">
         <v>192</v>
       </c>
     </row>
@@ -15871,4 +16107,232 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="30">
+      <c r="A25" s="14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="14"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="4"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="38" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>